<commit_message>
Some file has modified.
</commit_message>
<xml_diff>
--- a/Vizsgareme_POM_manuális_teszesetek.xlsx
+++ b/Vizsgareme_POM_manuális_teszesetek.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation_Tester\Vizsgaremek_POM\manuális_tesztesetek\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation_Tester\Vizsgaremek_POM\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -336,24 +336,12 @@
     <t>Ellenőrizze, hogy az adatküldés folyamatos és külső forrást használ.</t>
   </si>
   <si>
-    <t>1. https://en.wikipedia.org/wiki/Main_Page
-2.  "What"
-3. "is"
-4. "this"
-5. "Wikipedia"
-6. "captcha?"
-7. "captcha"</t>
-  </si>
-  <si>
     <t xml:space="preserve">1. A kívánt oldalon áll.
 2-3. Rákattintott a kereső gombra és új oldalon, új keresőmező nyílt.
 4. Ebbe a keresőmezőbe írta be az adatokat adatforrásból.
 5. Rákattintott a kereső gombra.
 6. Megjelentek a találatok és ezen webelemekben megkereste a "captcha" szót.
 </t>
-  </si>
-  <si>
-    <t>Az oldalon megjelent találatok releváns tartalommal rendelkeznek, mert sok tartalmazza a "captcha" szót.</t>
   </si>
   <si>
     <t>TC-08</t>
@@ -709,6 +697,17 @@
   </si>
   <si>
     <t>Ellenőrizze, hogy a megjelölt, megfelelő adatot találja meg, listaként járja be weboldalt és a találatokat számolja meg.</t>
+  </si>
+  <si>
+    <t>1. https://en.wikipedia.org/wiki/Main_Page
+4.  "What"
+4. "is"
+4. "this"
+4. "Wikipedia"
+4. "captcha?"</t>
+  </si>
+  <si>
+    <t>Az oldalon megjelent találatok releváns tartalommal rendelkeznek, mert a wnboldal tartalmazza a "captcha" szót.</t>
   </si>
 </sst>
 </file>
@@ -1260,9 +1259,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1"/>
@@ -1401,13 +1400,13 @@
         <v>45</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="H3" s="14" t="s">
         <v>53</v>
       </c>
       <c r="I3" s="12" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="J3" s="12" t="s">
         <v>55</v>
@@ -1501,7 +1500,7 @@
         <v>45</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="H5" s="13" t="s">
         <v>59</v>
@@ -1550,7 +1549,7 @@
         <v>45</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="H6" s="13" t="s">
         <v>68</v>
@@ -1599,7 +1598,7 @@
         <v>45</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="H7" s="13" t="s">
         <v>74</v>
@@ -1633,7 +1632,7 @@
         <v>77</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C8" s="12" t="s">
         <v>78</v>
@@ -1648,16 +1647,16 @@
         <v>45</v>
       </c>
       <c r="G8" s="12" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="H8" s="13" t="s">
         <v>80</v>
       </c>
       <c r="I8" s="13" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="J8" s="12" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="K8" s="13" t="s">
         <v>22</v>
@@ -1682,10 +1681,10 @@
         <v>81</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D9" s="12" t="s">
         <v>79</v>
@@ -1697,16 +1696,16 @@
         <v>45</v>
       </c>
       <c r="G9" s="12" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="H9" s="13" t="s">
         <v>80</v>
       </c>
       <c r="I9" s="13" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="J9" s="12" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="K9" s="13" t="s">
         <v>22</v>
@@ -1728,10 +1727,10 @@
     </row>
     <row r="10" spans="1:25" s="15" customFormat="1" ht="185.4" customHeight="1" thickTop="1" thickBot="1">
       <c r="A10" s="12" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C10" s="12" t="s">
         <v>82</v>
@@ -1746,16 +1745,16 @@
         <v>45</v>
       </c>
       <c r="G10" s="12" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H10" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="I10" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="I10" s="12" t="s">
-        <v>84</v>
-      </c>
       <c r="J10" s="12" t="s">
-        <v>85</v>
+        <v>152</v>
       </c>
       <c r="K10" s="13" t="s">
         <v>22</v>
@@ -1777,13 +1776,13 @@
     </row>
     <row r="11" spans="1:25" s="15" customFormat="1" ht="154.80000000000001" customHeight="1">
       <c r="A11" s="12" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D11" s="12" t="s">
         <v>79</v>
@@ -1795,16 +1794,16 @@
         <v>45</v>
       </c>
       <c r="G11" s="12" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="H11" s="13" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="I11" s="12" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="J11" s="12" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="K11" s="13" t="s">
         <v>22</v>
@@ -1826,13 +1825,13 @@
     </row>
     <row r="12" spans="1:25" s="15" customFormat="1" ht="199.8" customHeight="1">
       <c r="A12" s="12" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D12" s="12" t="s">
         <v>79</v>
@@ -1844,16 +1843,16 @@
         <v>45</v>
       </c>
       <c r="G12" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="H12" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="I12" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="J12" s="12" t="s">
         <v>101</v>
-      </c>
-      <c r="H12" s="13" t="s">
-        <v>100</v>
-      </c>
-      <c r="I12" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="J12" s="12" t="s">
-        <v>103</v>
       </c>
       <c r="K12" s="13" t="s">
         <v>22</v>
@@ -1875,13 +1874,13 @@
     </row>
     <row r="13" spans="1:25" s="15" customFormat="1" ht="196.2" customHeight="1">
       <c r="A13" s="12" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D13" s="12" t="s">
         <v>79</v>
@@ -1893,16 +1892,16 @@
         <v>45</v>
       </c>
       <c r="G13" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="H13" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="I13" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="H13" s="13" t="s">
+      <c r="J13" s="12" t="s">
         <v>108</v>
-      </c>
-      <c r="I13" s="12" t="s">
-        <v>109</v>
-      </c>
-      <c r="J13" s="12" t="s">
-        <v>110</v>
       </c>
       <c r="K13" s="13" t="s">
         <v>22</v>
@@ -1924,13 +1923,13 @@
     </row>
     <row r="14" spans="1:25" s="15" customFormat="1" ht="240" customHeight="1">
       <c r="A14" s="12" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D14" s="12" t="s">
         <v>79</v>
@@ -1942,16 +1941,16 @@
         <v>45</v>
       </c>
       <c r="G14" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="H14" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="I14" s="12" t="s">
         <v>114</v>
       </c>
-      <c r="H14" s="13" t="s">
-        <v>115</v>
-      </c>
-      <c r="I14" s="12" t="s">
+      <c r="J14" s="12" t="s">
         <v>116</v>
-      </c>
-      <c r="J14" s="12" t="s">
-        <v>118</v>
       </c>
       <c r="K14" s="13" t="s">
         <v>22</v>
@@ -1973,13 +1972,13 @@
     </row>
     <row r="15" spans="1:25" s="15" customFormat="1" ht="214.2" customHeight="1">
       <c r="A15" s="12" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D15" s="12" t="s">
         <v>79</v>
@@ -1991,16 +1990,16 @@
         <v>45</v>
       </c>
       <c r="G15" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="H15" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="I15" s="12" t="s">
         <v>135</v>
       </c>
-      <c r="H15" s="13" t="s">
+      <c r="J15" s="12" t="s">
         <v>136</v>
-      </c>
-      <c r="I15" s="12" t="s">
-        <v>137</v>
-      </c>
-      <c r="J15" s="12" t="s">
-        <v>138</v>
       </c>
       <c r="K15" s="13" t="s">
         <v>22</v>
@@ -2022,13 +2021,13 @@
     </row>
     <row r="16" spans="1:25" s="15" customFormat="1" ht="138.6" customHeight="1">
       <c r="A16" s="12" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D16" s="12" t="s">
         <v>79</v>
@@ -2040,16 +2039,16 @@
         <v>45</v>
       </c>
       <c r="G16" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="H16" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="I16" s="12" t="s">
         <v>125</v>
       </c>
-      <c r="H16" s="13" t="s">
+      <c r="J16" s="12" t="s">
         <v>126</v>
-      </c>
-      <c r="I16" s="12" t="s">
-        <v>127</v>
-      </c>
-      <c r="J16" s="12" t="s">
-        <v>128</v>
       </c>
       <c r="K16" s="13" t="s">
         <v>22</v>
@@ -2071,16 +2070,16 @@
     </row>
     <row r="17" spans="1:25" s="15" customFormat="1" ht="179.4" customHeight="1">
       <c r="A17" s="12" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E17" s="13" t="s">
         <v>43</v>
@@ -2089,16 +2088,16 @@
         <v>45</v>
       </c>
       <c r="G17" s="12" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="H17" s="13" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="I17" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="J17" s="12" t="s">
         <v>132</v>
-      </c>
-      <c r="J17" s="12" t="s">
-        <v>134</v>
       </c>
       <c r="K17" s="13" t="s">
         <v>22</v>

</xml_diff>

<commit_message>
Manual testcases has modified.
</commit_message>
<xml_diff>
--- a/Vizsgareme_POM_manuális_teszesetek.xlsx
+++ b/Vizsgareme_POM_manuális_teszesetek.xlsx
@@ -15,12 +15,15 @@
     <sheet name="tesztesetek (test case)" sheetId="1" r:id="rId1"/>
     <sheet name="hibák (bug)" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="IGEN">'tesztesetek (test case)'!$L$2</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="156">
   <si>
     <t>Azonosító (ID)</t>
   </si>
@@ -708,6 +711,15 @@
   </si>
   <si>
     <t>Az oldalon megjelent találatok releváns tartalommal rendelkeznek, mert a wnboldal tartalmazza a "captcha" szót.</t>
+  </si>
+  <si>
+    <t>Automatizálható a teszt?</t>
+  </si>
+  <si>
+    <t>NEM</t>
+  </si>
+  <si>
+    <t>IGEN</t>
   </si>
 </sst>
 </file>
@@ -759,7 +771,7 @@
       <charset val="238"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -775,6 +787,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF3F3F3"/>
+        <bgColor rgb="FFF3F3F3"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor rgb="FFF3F3F3"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor rgb="FFF3F3F3"/>
       </patternFill>
     </fill>
@@ -806,7 +830,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -849,6 +873,12 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
@@ -1257,11 +1287,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y1001"/>
+  <dimension ref="A1:Z1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L6" sqref="L6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1"/>
@@ -1277,11 +1307,12 @@
     <col min="9" max="9" width="24.8984375" customWidth="1"/>
     <col min="10" max="10" width="17" customWidth="1"/>
     <col min="11" max="11" width="16.19921875" customWidth="1"/>
-    <col min="12" max="12" width="24.59765625" customWidth="1"/>
-    <col min="15" max="15" width="20.8984375" customWidth="1"/>
+    <col min="12" max="12" width="16.8984375" customWidth="1"/>
+    <col min="13" max="13" width="24.59765625" customWidth="1"/>
+    <col min="16" max="16" width="20.8984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="46.8">
+    <row r="1" spans="1:26" ht="48" thickTop="1" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1316,12 +1347,14 @@
         <v>10</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="2"/>
       <c r="N1" s="2"/>
-      <c r="O1" s="11"/>
-      <c r="P1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="11"/>
       <c r="Q1" s="2"/>
       <c r="R1" s="2"/>
       <c r="S1" s="2"/>
@@ -1331,8 +1364,9 @@
       <c r="W1" s="2"/>
       <c r="X1" s="2"/>
       <c r="Y1" s="2"/>
-    </row>
-    <row r="2" spans="1:25" ht="60" customHeight="1" thickTop="1" thickBot="1">
+      <c r="Z1" s="2"/>
+    </row>
+    <row r="2" spans="1:26" ht="60" customHeight="1" thickTop="1" thickBot="1">
       <c r="A2" s="3" t="s">
         <v>12</v>
       </c>
@@ -1366,10 +1400,10 @@
       <c r="K2" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="L2" s="6"/>
-      <c r="M2" s="2"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="6"/>
       <c r="N2" s="2"/>
-      <c r="P2" s="2"/>
+      <c r="O2" s="2"/>
       <c r="Q2" s="2"/>
       <c r="R2" s="2"/>
       <c r="S2" s="2"/>
@@ -1379,8 +1413,9 @@
       <c r="W2" s="2"/>
       <c r="X2" s="2"/>
       <c r="Y2" s="2"/>
-    </row>
-    <row r="3" spans="1:25" ht="227.4" customHeight="1" thickTop="1" thickBot="1">
+      <c r="Z2" s="2"/>
+    </row>
+    <row r="3" spans="1:26" ht="227.4" customHeight="1" thickTop="1" thickBot="1">
       <c r="A3" s="12" t="s">
         <v>40</v>
       </c>
@@ -1414,10 +1449,12 @@
       <c r="K3" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="L3" s="12" t="s">
+      <c r="L3" s="17" t="s">
+        <v>154</v>
+      </c>
+      <c r="M3" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="M3" s="2"/>
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
       <c r="P3" s="2"/>
@@ -1430,8 +1467,9 @@
       <c r="W3" s="2"/>
       <c r="X3" s="2"/>
       <c r="Y3" s="2"/>
-    </row>
-    <row r="4" spans="1:25" ht="157.19999999999999" customHeight="1" thickTop="1" thickBot="1">
+      <c r="Z3" s="2"/>
+    </row>
+    <row r="4" spans="1:26" ht="157.19999999999999" customHeight="1" thickTop="1" thickBot="1">
       <c r="A4" s="12" t="s">
         <v>41</v>
       </c>
@@ -1465,8 +1503,10 @@
       <c r="K4" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="L4" s="12"/>
-      <c r="M4" s="2"/>
+      <c r="L4" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="M4" s="12"/>
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
       <c r="P4" s="2"/>
@@ -1479,8 +1519,9 @@
       <c r="W4" s="2"/>
       <c r="X4" s="2"/>
       <c r="Y4" s="2"/>
-    </row>
-    <row r="5" spans="1:25" ht="140.4" customHeight="1" thickTop="1" thickBot="1">
+      <c r="Z4" s="2"/>
+    </row>
+    <row r="5" spans="1:26" ht="140.4" customHeight="1" thickTop="1" thickBot="1">
       <c r="A5" s="12" t="s">
         <v>42</v>
       </c>
@@ -1514,8 +1555,10 @@
       <c r="K5" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="L5" s="7"/>
-      <c r="M5" s="2"/>
+      <c r="L5" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="M5" s="7"/>
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
       <c r="P5" s="2"/>
@@ -1528,8 +1571,9 @@
       <c r="W5" s="2"/>
       <c r="X5" s="2"/>
       <c r="Y5" s="2"/>
-    </row>
-    <row r="6" spans="1:25" ht="156" customHeight="1" thickTop="1" thickBot="1">
+      <c r="Z5" s="2"/>
+    </row>
+    <row r="6" spans="1:26" ht="156" customHeight="1" thickTop="1" thickBot="1">
       <c r="A6" s="12" t="s">
         <v>62</v>
       </c>
@@ -1563,8 +1607,10 @@
       <c r="K6" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="L6" s="7"/>
-      <c r="M6" s="2"/>
+      <c r="L6" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="M6" s="7"/>
       <c r="N6" s="2"/>
       <c r="O6" s="2"/>
       <c r="P6" s="2"/>
@@ -1577,8 +1623,9 @@
       <c r="W6" s="2"/>
       <c r="X6" s="2"/>
       <c r="Y6" s="2"/>
-    </row>
-    <row r="7" spans="1:25" ht="243" customHeight="1" thickTop="1" thickBot="1">
+      <c r="Z6" s="2"/>
+    </row>
+    <row r="7" spans="1:26" ht="243" customHeight="1" thickTop="1" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>71</v>
       </c>
@@ -1612,8 +1659,10 @@
       <c r="K7" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="L7" s="7"/>
-      <c r="M7" s="2"/>
+      <c r="L7" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="M7" s="7"/>
       <c r="N7" s="2"/>
       <c r="O7" s="2"/>
       <c r="P7" s="2"/>
@@ -1626,8 +1675,9 @@
       <c r="W7" s="2"/>
       <c r="X7" s="2"/>
       <c r="Y7" s="2"/>
-    </row>
-    <row r="8" spans="1:25" s="15" customFormat="1" ht="204" customHeight="1" thickTop="1" thickBot="1">
+      <c r="Z7" s="2"/>
+    </row>
+    <row r="8" spans="1:26" s="15" customFormat="1" ht="204" customHeight="1" thickTop="1" thickBot="1">
       <c r="A8" s="12" t="s">
         <v>77</v>
       </c>
@@ -1661,8 +1711,10 @@
       <c r="K8" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="L8" s="12"/>
-      <c r="M8" s="2"/>
+      <c r="L8" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="M8" s="12"/>
       <c r="N8" s="2"/>
       <c r="O8" s="2"/>
       <c r="P8" s="2"/>
@@ -1675,8 +1727,9 @@
       <c r="W8" s="2"/>
       <c r="X8" s="2"/>
       <c r="Y8" s="2"/>
-    </row>
-    <row r="9" spans="1:25" s="15" customFormat="1" ht="204" customHeight="1" thickTop="1" thickBot="1">
+      <c r="Z8" s="2"/>
+    </row>
+    <row r="9" spans="1:26" s="15" customFormat="1" ht="204" customHeight="1" thickTop="1" thickBot="1">
       <c r="A9" s="12" t="s">
         <v>81</v>
       </c>
@@ -1710,8 +1763,10 @@
       <c r="K9" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="L9" s="12"/>
-      <c r="M9" s="2"/>
+      <c r="L9" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="M9" s="12"/>
       <c r="N9" s="2"/>
       <c r="O9" s="2"/>
       <c r="P9" s="2"/>
@@ -1724,8 +1779,9 @@
       <c r="W9" s="2"/>
       <c r="X9" s="2"/>
       <c r="Y9" s="2"/>
-    </row>
-    <row r="10" spans="1:25" s="15" customFormat="1" ht="185.4" customHeight="1" thickTop="1" thickBot="1">
+      <c r="Z9" s="2"/>
+    </row>
+    <row r="10" spans="1:26" s="15" customFormat="1" ht="185.4" customHeight="1" thickTop="1" thickBot="1">
       <c r="A10" s="12" t="s">
         <v>84</v>
       </c>
@@ -1759,8 +1815,10 @@
       <c r="K10" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="L10" s="12"/>
-      <c r="M10" s="2"/>
+      <c r="L10" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="M10" s="12"/>
       <c r="N10" s="2"/>
       <c r="O10" s="2"/>
       <c r="P10" s="2"/>
@@ -1773,8 +1831,9 @@
       <c r="W10" s="2"/>
       <c r="X10" s="2"/>
       <c r="Y10" s="2"/>
-    </row>
-    <row r="11" spans="1:25" s="15" customFormat="1" ht="154.80000000000001" customHeight="1">
+      <c r="Z10" s="2"/>
+    </row>
+    <row r="11" spans="1:26" s="15" customFormat="1" ht="154.80000000000001" customHeight="1" thickTop="1" thickBot="1">
       <c r="A11" s="12" t="s">
         <v>89</v>
       </c>
@@ -1808,8 +1867,10 @@
       <c r="K11" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="L11" s="12"/>
-      <c r="M11" s="2"/>
+      <c r="L11" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="M11" s="12"/>
       <c r="N11" s="2"/>
       <c r="O11" s="2"/>
       <c r="P11" s="2"/>
@@ -1822,8 +1883,9 @@
       <c r="W11" s="2"/>
       <c r="X11" s="2"/>
       <c r="Y11" s="2"/>
-    </row>
-    <row r="12" spans="1:25" s="15" customFormat="1" ht="199.8" customHeight="1">
+      <c r="Z11" s="2"/>
+    </row>
+    <row r="12" spans="1:26" s="15" customFormat="1" ht="199.8" customHeight="1" thickTop="1" thickBot="1">
       <c r="A12" s="12" t="s">
         <v>102</v>
       </c>
@@ -1857,8 +1919,10 @@
       <c r="K12" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="L12" s="12"/>
-      <c r="M12" s="2"/>
+      <c r="L12" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="M12" s="12"/>
       <c r="N12" s="2"/>
       <c r="O12" s="2"/>
       <c r="P12" s="2"/>
@@ -1871,8 +1935,9 @@
       <c r="W12" s="2"/>
       <c r="X12" s="2"/>
       <c r="Y12" s="2"/>
-    </row>
-    <row r="13" spans="1:25" s="15" customFormat="1" ht="196.2" customHeight="1">
+      <c r="Z12" s="2"/>
+    </row>
+    <row r="13" spans="1:26" s="15" customFormat="1" ht="196.2" customHeight="1" thickTop="1" thickBot="1">
       <c r="A13" s="12" t="s">
         <v>110</v>
       </c>
@@ -1906,8 +1971,10 @@
       <c r="K13" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="L13" s="12"/>
-      <c r="M13" s="2"/>
+      <c r="L13" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="M13" s="12"/>
       <c r="N13" s="2"/>
       <c r="O13" s="2"/>
       <c r="P13" s="2"/>
@@ -1920,8 +1987,9 @@
       <c r="W13" s="2"/>
       <c r="X13" s="2"/>
       <c r="Y13" s="2"/>
-    </row>
-    <row r="14" spans="1:25" s="15" customFormat="1" ht="240" customHeight="1">
+      <c r="Z13" s="2"/>
+    </row>
+    <row r="14" spans="1:26" s="15" customFormat="1" ht="240" customHeight="1" thickTop="1" thickBot="1">
       <c r="A14" s="12" t="s">
         <v>117</v>
       </c>
@@ -1955,8 +2023,10 @@
       <c r="K14" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="L14" s="12"/>
-      <c r="M14" s="2"/>
+      <c r="L14" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="M14" s="12"/>
       <c r="N14" s="2"/>
       <c r="O14" s="2"/>
       <c r="P14" s="2"/>
@@ -1969,8 +2039,9 @@
       <c r="W14" s="2"/>
       <c r="X14" s="2"/>
       <c r="Y14" s="2"/>
-    </row>
-    <row r="15" spans="1:25" s="15" customFormat="1" ht="214.2" customHeight="1">
+      <c r="Z14" s="2"/>
+    </row>
+    <row r="15" spans="1:26" s="15" customFormat="1" ht="214.2" customHeight="1" thickTop="1" thickBot="1">
       <c r="A15" s="12" t="s">
         <v>120</v>
       </c>
@@ -2004,8 +2075,10 @@
       <c r="K15" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="L15" s="12"/>
-      <c r="M15" s="2"/>
+      <c r="L15" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="M15" s="12"/>
       <c r="N15" s="2"/>
       <c r="O15" s="2"/>
       <c r="P15" s="2"/>
@@ -2018,8 +2091,9 @@
       <c r="W15" s="2"/>
       <c r="X15" s="2"/>
       <c r="Y15" s="2"/>
-    </row>
-    <row r="16" spans="1:25" s="15" customFormat="1" ht="138.6" customHeight="1">
+      <c r="Z15" s="2"/>
+    </row>
+    <row r="16" spans="1:26" s="15" customFormat="1" ht="138.6" customHeight="1" thickTop="1" thickBot="1">
       <c r="A16" s="12" t="s">
         <v>127</v>
       </c>
@@ -2053,8 +2127,10 @@
       <c r="K16" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="L16" s="12"/>
-      <c r="M16" s="2"/>
+      <c r="L16" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="M16" s="12"/>
       <c r="N16" s="2"/>
       <c r="O16" s="2"/>
       <c r="P16" s="2"/>
@@ -2067,8 +2143,9 @@
       <c r="W16" s="2"/>
       <c r="X16" s="2"/>
       <c r="Y16" s="2"/>
-    </row>
-    <row r="17" spans="1:25" s="15" customFormat="1" ht="179.4" customHeight="1">
+      <c r="Z16" s="2"/>
+    </row>
+    <row r="17" spans="1:26" s="15" customFormat="1" ht="179.4" customHeight="1" thickTop="1" thickBot="1">
       <c r="A17" s="12" t="s">
         <v>143</v>
       </c>
@@ -2102,8 +2179,10 @@
       <c r="K17" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="L17" s="12"/>
-      <c r="M17" s="2"/>
+      <c r="L17" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="M17" s="12"/>
       <c r="N17" s="2"/>
       <c r="O17" s="2"/>
       <c r="P17" s="2"/>
@@ -2116,8 +2195,9 @@
       <c r="W17" s="2"/>
       <c r="X17" s="2"/>
       <c r="Y17" s="2"/>
-    </row>
-    <row r="18" spans="1:25" ht="60" customHeight="1">
+      <c r="Z17" s="2"/>
+    </row>
+    <row r="18" spans="1:26" ht="60" customHeight="1" thickTop="1" thickBot="1">
       <c r="A18" s="7"/>
       <c r="B18" s="7"/>
       <c r="C18" s="7"/>
@@ -2129,8 +2209,8 @@
       <c r="I18" s="7"/>
       <c r="J18" s="7"/>
       <c r="K18" s="8"/>
-      <c r="L18" s="7"/>
-      <c r="M18" s="2"/>
+      <c r="L18" s="9"/>
+      <c r="M18" s="7"/>
       <c r="N18" s="2"/>
       <c r="O18" s="2"/>
       <c r="P18" s="2"/>
@@ -2143,8 +2223,9 @@
       <c r="W18" s="2"/>
       <c r="X18" s="2"/>
       <c r="Y18" s="2"/>
-    </row>
-    <row r="19" spans="1:25" ht="60" customHeight="1">
+      <c r="Z18" s="2"/>
+    </row>
+    <row r="19" spans="1:26" ht="60" customHeight="1" thickTop="1" thickBot="1">
       <c r="A19" s="7"/>
       <c r="B19" s="7"/>
       <c r="C19" s="7"/>
@@ -2156,8 +2237,8 @@
       <c r="I19" s="7"/>
       <c r="J19" s="7"/>
       <c r="K19" s="8"/>
-      <c r="L19" s="7"/>
-      <c r="M19" s="2"/>
+      <c r="L19" s="9"/>
+      <c r="M19" s="7"/>
       <c r="N19" s="2"/>
       <c r="O19" s="2"/>
       <c r="P19" s="2"/>
@@ -2170,8 +2251,9 @@
       <c r="W19" s="2"/>
       <c r="X19" s="2"/>
       <c r="Y19" s="2"/>
-    </row>
-    <row r="20" spans="1:25" ht="60" customHeight="1">
+      <c r="Z19" s="2"/>
+    </row>
+    <row r="20" spans="1:26" ht="60" customHeight="1" thickTop="1" thickBot="1">
       <c r="A20" s="7"/>
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
@@ -2183,8 +2265,8 @@
       <c r="I20" s="7"/>
       <c r="J20" s="7"/>
       <c r="K20" s="8"/>
-      <c r="L20" s="7"/>
-      <c r="M20" s="2"/>
+      <c r="L20" s="9"/>
+      <c r="M20" s="7"/>
       <c r="N20" s="2"/>
       <c r="O20" s="2"/>
       <c r="P20" s="2"/>
@@ -2197,8 +2279,9 @@
       <c r="W20" s="2"/>
       <c r="X20" s="2"/>
       <c r="Y20" s="2"/>
-    </row>
-    <row r="21" spans="1:25" ht="60" customHeight="1">
+      <c r="Z20" s="2"/>
+    </row>
+    <row r="21" spans="1:26" ht="60" customHeight="1" thickTop="1" thickBot="1">
       <c r="A21" s="7"/>
       <c r="B21" s="7"/>
       <c r="C21" s="7"/>
@@ -2210,8 +2293,8 @@
       <c r="I21" s="7"/>
       <c r="J21" s="7"/>
       <c r="K21" s="8"/>
-      <c r="L21" s="7"/>
-      <c r="M21" s="2"/>
+      <c r="L21" s="9"/>
+      <c r="M21" s="7"/>
       <c r="N21" s="2"/>
       <c r="O21" s="2"/>
       <c r="P21" s="2"/>
@@ -2224,8 +2307,9 @@
       <c r="W21" s="2"/>
       <c r="X21" s="2"/>
       <c r="Y21" s="2"/>
-    </row>
-    <row r="22" spans="1:25" ht="60" customHeight="1">
+      <c r="Z21" s="2"/>
+    </row>
+    <row r="22" spans="1:26" ht="60" customHeight="1" thickTop="1" thickBot="1">
       <c r="A22" s="7"/>
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
@@ -2237,8 +2321,8 @@
       <c r="I22" s="7"/>
       <c r="J22" s="7"/>
       <c r="K22" s="8"/>
-      <c r="L22" s="7"/>
-      <c r="M22" s="2"/>
+      <c r="L22" s="9"/>
+      <c r="M22" s="7"/>
       <c r="N22" s="2"/>
       <c r="O22" s="2"/>
       <c r="P22" s="2"/>
@@ -2251,8 +2335,9 @@
       <c r="W22" s="2"/>
       <c r="X22" s="2"/>
       <c r="Y22" s="2"/>
-    </row>
-    <row r="23" spans="1:25" ht="60" customHeight="1">
+      <c r="Z22" s="2"/>
+    </row>
+    <row r="23" spans="1:26" ht="60" customHeight="1" thickTop="1" thickBot="1">
       <c r="A23" s="7"/>
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
@@ -2264,8 +2349,8 @@
       <c r="I23" s="7"/>
       <c r="J23" s="7"/>
       <c r="K23" s="8"/>
-      <c r="L23" s="7"/>
-      <c r="M23" s="2"/>
+      <c r="L23" s="9"/>
+      <c r="M23" s="7"/>
       <c r="N23" s="2"/>
       <c r="O23" s="2"/>
       <c r="P23" s="2"/>
@@ -2278,8 +2363,9 @@
       <c r="W23" s="2"/>
       <c r="X23" s="2"/>
       <c r="Y23" s="2"/>
-    </row>
-    <row r="24" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z23" s="2"/>
+    </row>
+    <row r="24" spans="1:26" ht="15.75" customHeight="1" thickTop="1">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -2305,8 +2391,9 @@
       <c r="W24" s="2"/>
       <c r="X24" s="2"/>
       <c r="Y24" s="2"/>
-    </row>
-    <row r="25" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z24" s="2"/>
+    </row>
+    <row r="25" spans="1:26" ht="15.75" customHeight="1">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -2332,8 +2419,9 @@
       <c r="W25" s="2"/>
       <c r="X25" s="2"/>
       <c r="Y25" s="2"/>
-    </row>
-    <row r="26" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z25" s="2"/>
+    </row>
+    <row r="26" spans="1:26" ht="15.75" customHeight="1">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -2359,8 +2447,9 @@
       <c r="W26" s="2"/>
       <c r="X26" s="2"/>
       <c r="Y26" s="2"/>
-    </row>
-    <row r="27" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z26" s="2"/>
+    </row>
+    <row r="27" spans="1:26" ht="15.75" customHeight="1">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -2386,8 +2475,9 @@
       <c r="W27" s="2"/>
       <c r="X27" s="2"/>
       <c r="Y27" s="2"/>
-    </row>
-    <row r="28" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z27" s="2"/>
+    </row>
+    <row r="28" spans="1:26" ht="15.75" customHeight="1">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -2413,8 +2503,9 @@
       <c r="W28" s="2"/>
       <c r="X28" s="2"/>
       <c r="Y28" s="2"/>
-    </row>
-    <row r="29" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z28" s="2"/>
+    </row>
+    <row r="29" spans="1:26" ht="15.75" customHeight="1">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -2440,8 +2531,9 @@
       <c r="W29" s="2"/>
       <c r="X29" s="2"/>
       <c r="Y29" s="2"/>
-    </row>
-    <row r="30" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z29" s="2"/>
+    </row>
+    <row r="30" spans="1:26" ht="15.75" customHeight="1">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
@@ -2467,8 +2559,9 @@
       <c r="W30" s="2"/>
       <c r="X30" s="2"/>
       <c r="Y30" s="2"/>
-    </row>
-    <row r="31" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z30" s="2"/>
+    </row>
+    <row r="31" spans="1:26" ht="15.75" customHeight="1">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
@@ -2494,8 +2587,9 @@
       <c r="W31" s="2"/>
       <c r="X31" s="2"/>
       <c r="Y31" s="2"/>
-    </row>
-    <row r="32" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z31" s="2"/>
+    </row>
+    <row r="32" spans="1:26" ht="15.75" customHeight="1">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
@@ -2521,8 +2615,9 @@
       <c r="W32" s="2"/>
       <c r="X32" s="2"/>
       <c r="Y32" s="2"/>
-    </row>
-    <row r="33" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z32" s="2"/>
+    </row>
+    <row r="33" spans="1:26" ht="15.75" customHeight="1">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
@@ -2548,8 +2643,9 @@
       <c r="W33" s="2"/>
       <c r="X33" s="2"/>
       <c r="Y33" s="2"/>
-    </row>
-    <row r="34" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z33" s="2"/>
+    </row>
+    <row r="34" spans="1:26" ht="15.75" customHeight="1">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
@@ -2575,8 +2671,9 @@
       <c r="W34" s="2"/>
       <c r="X34" s="2"/>
       <c r="Y34" s="2"/>
-    </row>
-    <row r="35" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z34" s="2"/>
+    </row>
+    <row r="35" spans="1:26" ht="15.75" customHeight="1">
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
@@ -2602,8 +2699,9 @@
       <c r="W35" s="2"/>
       <c r="X35" s="2"/>
       <c r="Y35" s="2"/>
-    </row>
-    <row r="36" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z35" s="2"/>
+    </row>
+    <row r="36" spans="1:26" ht="15.75" customHeight="1">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
@@ -2629,8 +2727,9 @@
       <c r="W36" s="2"/>
       <c r="X36" s="2"/>
       <c r="Y36" s="2"/>
-    </row>
-    <row r="37" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z36" s="2"/>
+    </row>
+    <row r="37" spans="1:26" ht="15.75" customHeight="1">
       <c r="A37" s="2"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
@@ -2656,8 +2755,9 @@
       <c r="W37" s="2"/>
       <c r="X37" s="2"/>
       <c r="Y37" s="2"/>
-    </row>
-    <row r="38" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z37" s="2"/>
+    </row>
+    <row r="38" spans="1:26" ht="15.75" customHeight="1">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
@@ -2683,8 +2783,9 @@
       <c r="W38" s="2"/>
       <c r="X38" s="2"/>
       <c r="Y38" s="2"/>
-    </row>
-    <row r="39" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z38" s="2"/>
+    </row>
+    <row r="39" spans="1:26" ht="15.75" customHeight="1">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
@@ -2710,8 +2811,9 @@
       <c r="W39" s="2"/>
       <c r="X39" s="2"/>
       <c r="Y39" s="2"/>
-    </row>
-    <row r="40" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z39" s="2"/>
+    </row>
+    <row r="40" spans="1:26" ht="15.75" customHeight="1">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
@@ -2737,8 +2839,9 @@
       <c r="W40" s="2"/>
       <c r="X40" s="2"/>
       <c r="Y40" s="2"/>
-    </row>
-    <row r="41" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z40" s="2"/>
+    </row>
+    <row r="41" spans="1:26" ht="15.75" customHeight="1">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
@@ -2764,8 +2867,9 @@
       <c r="W41" s="2"/>
       <c r="X41" s="2"/>
       <c r="Y41" s="2"/>
-    </row>
-    <row r="42" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z41" s="2"/>
+    </row>
+    <row r="42" spans="1:26" ht="15.75" customHeight="1">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
@@ -2791,8 +2895,9 @@
       <c r="W42" s="2"/>
       <c r="X42" s="2"/>
       <c r="Y42" s="2"/>
-    </row>
-    <row r="43" spans="1:25" ht="15.75" customHeight="1" thickBot="1">
+      <c r="Z42" s="2"/>
+    </row>
+    <row r="43" spans="1:26" ht="15.75" customHeight="1" thickBot="1">
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
@@ -2818,8 +2923,9 @@
       <c r="W43" s="2"/>
       <c r="X43" s="2"/>
       <c r="Y43" s="2"/>
-    </row>
-    <row r="44" spans="1:25" ht="15.75" customHeight="1" thickTop="1" thickBot="1">
+      <c r="Z43" s="2"/>
+    </row>
+    <row r="44" spans="1:26" ht="15.75" customHeight="1" thickTop="1" thickBot="1">
       <c r="A44" s="2"/>
       <c r="B44" s="12"/>
       <c r="C44" s="2"/>
@@ -2845,8 +2951,9 @@
       <c r="W44" s="2"/>
       <c r="X44" s="2"/>
       <c r="Y44" s="2"/>
-    </row>
-    <row r="45" spans="1:25" ht="15.75" customHeight="1" thickTop="1">
+      <c r="Z44" s="2"/>
+    </row>
+    <row r="45" spans="1:26" ht="15.75" customHeight="1" thickTop="1">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
@@ -2872,8 +2979,9 @@
       <c r="W45" s="2"/>
       <c r="X45" s="2"/>
       <c r="Y45" s="2"/>
-    </row>
-    <row r="46" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z45" s="2"/>
+    </row>
+    <row r="46" spans="1:26" ht="15.75" customHeight="1">
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
@@ -2899,8 +3007,9 @@
       <c r="W46" s="2"/>
       <c r="X46" s="2"/>
       <c r="Y46" s="2"/>
-    </row>
-    <row r="47" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z46" s="2"/>
+    </row>
+    <row r="47" spans="1:26" ht="15.75" customHeight="1">
       <c r="A47" s="2"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
@@ -2926,8 +3035,9 @@
       <c r="W47" s="2"/>
       <c r="X47" s="2"/>
       <c r="Y47" s="2"/>
-    </row>
-    <row r="48" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z47" s="2"/>
+    </row>
+    <row r="48" spans="1:26" ht="15.75" customHeight="1">
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
@@ -2953,8 +3063,9 @@
       <c r="W48" s="2"/>
       <c r="X48" s="2"/>
       <c r="Y48" s="2"/>
-    </row>
-    <row r="49" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z48" s="2"/>
+    </row>
+    <row r="49" spans="1:26" ht="15.75" customHeight="1">
       <c r="A49" s="2"/>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
@@ -2980,8 +3091,9 @@
       <c r="W49" s="2"/>
       <c r="X49" s="2"/>
       <c r="Y49" s="2"/>
-    </row>
-    <row r="50" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z49" s="2"/>
+    </row>
+    <row r="50" spans="1:26" ht="15.75" customHeight="1">
       <c r="A50" s="2"/>
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
@@ -3007,8 +3119,9 @@
       <c r="W50" s="2"/>
       <c r="X50" s="2"/>
       <c r="Y50" s="2"/>
-    </row>
-    <row r="51" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z50" s="2"/>
+    </row>
+    <row r="51" spans="1:26" ht="15.75" customHeight="1">
       <c r="A51" s="2"/>
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
@@ -3034,8 +3147,9 @@
       <c r="W51" s="2"/>
       <c r="X51" s="2"/>
       <c r="Y51" s="2"/>
-    </row>
-    <row r="52" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z51" s="2"/>
+    </row>
+    <row r="52" spans="1:26" ht="15.75" customHeight="1">
       <c r="A52" s="2"/>
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
@@ -3061,8 +3175,9 @@
       <c r="W52" s="2"/>
       <c r="X52" s="2"/>
       <c r="Y52" s="2"/>
-    </row>
-    <row r="53" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z52" s="2"/>
+    </row>
+    <row r="53" spans="1:26" ht="15.75" customHeight="1">
       <c r="A53" s="2"/>
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
@@ -3088,8 +3203,9 @@
       <c r="W53" s="2"/>
       <c r="X53" s="2"/>
       <c r="Y53" s="2"/>
-    </row>
-    <row r="54" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z53" s="2"/>
+    </row>
+    <row r="54" spans="1:26" ht="15.75" customHeight="1">
       <c r="A54" s="2"/>
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
@@ -3115,8 +3231,9 @@
       <c r="W54" s="2"/>
       <c r="X54" s="2"/>
       <c r="Y54" s="2"/>
-    </row>
-    <row r="55" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z54" s="2"/>
+    </row>
+    <row r="55" spans="1:26" ht="15.75" customHeight="1">
       <c r="A55" s="2"/>
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
@@ -3142,8 +3259,9 @@
       <c r="W55" s="2"/>
       <c r="X55" s="2"/>
       <c r="Y55" s="2"/>
-    </row>
-    <row r="56" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z55" s="2"/>
+    </row>
+    <row r="56" spans="1:26" ht="15.75" customHeight="1">
       <c r="A56" s="2"/>
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
@@ -3169,8 +3287,9 @@
       <c r="W56" s="2"/>
       <c r="X56" s="2"/>
       <c r="Y56" s="2"/>
-    </row>
-    <row r="57" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z56" s="2"/>
+    </row>
+    <row r="57" spans="1:26" ht="15.75" customHeight="1">
       <c r="A57" s="2"/>
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
@@ -3196,8 +3315,9 @@
       <c r="W57" s="2"/>
       <c r="X57" s="2"/>
       <c r="Y57" s="2"/>
-    </row>
-    <row r="58" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z57" s="2"/>
+    </row>
+    <row r="58" spans="1:26" ht="15.75" customHeight="1">
       <c r="A58" s="2"/>
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
@@ -3223,8 +3343,9 @@
       <c r="W58" s="2"/>
       <c r="X58" s="2"/>
       <c r="Y58" s="2"/>
-    </row>
-    <row r="59" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z58" s="2"/>
+    </row>
+    <row r="59" spans="1:26" ht="15.75" customHeight="1">
       <c r="A59" s="2"/>
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
@@ -3250,8 +3371,9 @@
       <c r="W59" s="2"/>
       <c r="X59" s="2"/>
       <c r="Y59" s="2"/>
-    </row>
-    <row r="60" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z59" s="2"/>
+    </row>
+    <row r="60" spans="1:26" ht="15.75" customHeight="1">
       <c r="A60" s="2"/>
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
@@ -3277,8 +3399,9 @@
       <c r="W60" s="2"/>
       <c r="X60" s="2"/>
       <c r="Y60" s="2"/>
-    </row>
-    <row r="61" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z60" s="2"/>
+    </row>
+    <row r="61" spans="1:26" ht="15.75" customHeight="1">
       <c r="A61" s="2"/>
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
@@ -3304,8 +3427,9 @@
       <c r="W61" s="2"/>
       <c r="X61" s="2"/>
       <c r="Y61" s="2"/>
-    </row>
-    <row r="62" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z61" s="2"/>
+    </row>
+    <row r="62" spans="1:26" ht="15.75" customHeight="1">
       <c r="A62" s="2"/>
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
@@ -3331,8 +3455,9 @@
       <c r="W62" s="2"/>
       <c r="X62" s="2"/>
       <c r="Y62" s="2"/>
-    </row>
-    <row r="63" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z62" s="2"/>
+    </row>
+    <row r="63" spans="1:26" ht="15.75" customHeight="1">
       <c r="A63" s="2"/>
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
@@ -3358,8 +3483,9 @@
       <c r="W63" s="2"/>
       <c r="X63" s="2"/>
       <c r="Y63" s="2"/>
-    </row>
-    <row r="64" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z63" s="2"/>
+    </row>
+    <row r="64" spans="1:26" ht="15.75" customHeight="1">
       <c r="A64" s="2"/>
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
@@ -3385,8 +3511,9 @@
       <c r="W64" s="2"/>
       <c r="X64" s="2"/>
       <c r="Y64" s="2"/>
-    </row>
-    <row r="65" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z64" s="2"/>
+    </row>
+    <row r="65" spans="1:26" ht="15.75" customHeight="1">
       <c r="A65" s="2"/>
       <c r="B65" s="2"/>
       <c r="C65" s="2"/>
@@ -3412,8 +3539,9 @@
       <c r="W65" s="2"/>
       <c r="X65" s="2"/>
       <c r="Y65" s="2"/>
-    </row>
-    <row r="66" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z65" s="2"/>
+    </row>
+    <row r="66" spans="1:26" ht="15.75" customHeight="1">
       <c r="A66" s="2"/>
       <c r="B66" s="2"/>
       <c r="C66" s="2"/>
@@ -3439,8 +3567,9 @@
       <c r="W66" s="2"/>
       <c r="X66" s="2"/>
       <c r="Y66" s="2"/>
-    </row>
-    <row r="67" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z66" s="2"/>
+    </row>
+    <row r="67" spans="1:26" ht="15.75" customHeight="1">
       <c r="A67" s="2"/>
       <c r="B67" s="2"/>
       <c r="C67" s="2"/>
@@ -3466,8 +3595,9 @@
       <c r="W67" s="2"/>
       <c r="X67" s="2"/>
       <c r="Y67" s="2"/>
-    </row>
-    <row r="68" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z67" s="2"/>
+    </row>
+    <row r="68" spans="1:26" ht="15.75" customHeight="1">
       <c r="A68" s="2"/>
       <c r="B68" s="2"/>
       <c r="C68" s="2"/>
@@ -3493,8 +3623,9 @@
       <c r="W68" s="2"/>
       <c r="X68" s="2"/>
       <c r="Y68" s="2"/>
-    </row>
-    <row r="69" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z68" s="2"/>
+    </row>
+    <row r="69" spans="1:26" ht="15.75" customHeight="1">
       <c r="A69" s="2"/>
       <c r="B69" s="2"/>
       <c r="C69" s="2"/>
@@ -3520,8 +3651,9 @@
       <c r="W69" s="2"/>
       <c r="X69" s="2"/>
       <c r="Y69" s="2"/>
-    </row>
-    <row r="70" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z69" s="2"/>
+    </row>
+    <row r="70" spans="1:26" ht="15.75" customHeight="1">
       <c r="A70" s="2"/>
       <c r="B70" s="2"/>
       <c r="C70" s="2"/>
@@ -3547,8 +3679,9 @@
       <c r="W70" s="2"/>
       <c r="X70" s="2"/>
       <c r="Y70" s="2"/>
-    </row>
-    <row r="71" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z70" s="2"/>
+    </row>
+    <row r="71" spans="1:26" ht="15.75" customHeight="1">
       <c r="A71" s="2"/>
       <c r="B71" s="2"/>
       <c r="C71" s="2"/>
@@ -3574,8 +3707,9 @@
       <c r="W71" s="2"/>
       <c r="X71" s="2"/>
       <c r="Y71" s="2"/>
-    </row>
-    <row r="72" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z71" s="2"/>
+    </row>
+    <row r="72" spans="1:26" ht="15.75" customHeight="1">
       <c r="A72" s="2"/>
       <c r="B72" s="2"/>
       <c r="C72" s="2"/>
@@ -3601,8 +3735,9 @@
       <c r="W72" s="2"/>
       <c r="X72" s="2"/>
       <c r="Y72" s="2"/>
-    </row>
-    <row r="73" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z72" s="2"/>
+    </row>
+    <row r="73" spans="1:26" ht="15.75" customHeight="1">
       <c r="A73" s="2"/>
       <c r="B73" s="2"/>
       <c r="C73" s="2"/>
@@ -3628,8 +3763,9 @@
       <c r="W73" s="2"/>
       <c r="X73" s="2"/>
       <c r="Y73" s="2"/>
-    </row>
-    <row r="74" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z73" s="2"/>
+    </row>
+    <row r="74" spans="1:26" ht="15.75" customHeight="1">
       <c r="A74" s="2"/>
       <c r="B74" s="2"/>
       <c r="C74" s="2"/>
@@ -3655,8 +3791,9 @@
       <c r="W74" s="2"/>
       <c r="X74" s="2"/>
       <c r="Y74" s="2"/>
-    </row>
-    <row r="75" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z74" s="2"/>
+    </row>
+    <row r="75" spans="1:26" ht="15.75" customHeight="1">
       <c r="A75" s="2"/>
       <c r="B75" s="2"/>
       <c r="C75" s="2"/>
@@ -3682,8 +3819,9 @@
       <c r="W75" s="2"/>
       <c r="X75" s="2"/>
       <c r="Y75" s="2"/>
-    </row>
-    <row r="76" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z75" s="2"/>
+    </row>
+    <row r="76" spans="1:26" ht="15.75" customHeight="1">
       <c r="A76" s="2"/>
       <c r="B76" s="2"/>
       <c r="C76" s="2"/>
@@ -3709,8 +3847,9 @@
       <c r="W76" s="2"/>
       <c r="X76" s="2"/>
       <c r="Y76" s="2"/>
-    </row>
-    <row r="77" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z76" s="2"/>
+    </row>
+    <row r="77" spans="1:26" ht="15.75" customHeight="1">
       <c r="A77" s="2"/>
       <c r="B77" s="2"/>
       <c r="C77" s="2"/>
@@ -3736,8 +3875,9 @@
       <c r="W77" s="2"/>
       <c r="X77" s="2"/>
       <c r="Y77" s="2"/>
-    </row>
-    <row r="78" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z77" s="2"/>
+    </row>
+    <row r="78" spans="1:26" ht="15.75" customHeight="1">
       <c r="A78" s="2"/>
       <c r="B78" s="2"/>
       <c r="C78" s="2"/>
@@ -3763,8 +3903,9 @@
       <c r="W78" s="2"/>
       <c r="X78" s="2"/>
       <c r="Y78" s="2"/>
-    </row>
-    <row r="79" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z78" s="2"/>
+    </row>
+    <row r="79" spans="1:26" ht="15.75" customHeight="1">
       <c r="A79" s="2"/>
       <c r="B79" s="2"/>
       <c r="C79" s="2"/>
@@ -3790,8 +3931,9 @@
       <c r="W79" s="2"/>
       <c r="X79" s="2"/>
       <c r="Y79" s="2"/>
-    </row>
-    <row r="80" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z79" s="2"/>
+    </row>
+    <row r="80" spans="1:26" ht="15.75" customHeight="1">
       <c r="A80" s="2"/>
       <c r="B80" s="2"/>
       <c r="C80" s="2"/>
@@ -3817,8 +3959,9 @@
       <c r="W80" s="2"/>
       <c r="X80" s="2"/>
       <c r="Y80" s="2"/>
-    </row>
-    <row r="81" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z80" s="2"/>
+    </row>
+    <row r="81" spans="1:26" ht="15.75" customHeight="1">
       <c r="A81" s="2"/>
       <c r="B81" s="2"/>
       <c r="C81" s="2"/>
@@ -3844,8 +3987,9 @@
       <c r="W81" s="2"/>
       <c r="X81" s="2"/>
       <c r="Y81" s="2"/>
-    </row>
-    <row r="82" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z81" s="2"/>
+    </row>
+    <row r="82" spans="1:26" ht="15.75" customHeight="1">
       <c r="A82" s="2"/>
       <c r="B82" s="2"/>
       <c r="C82" s="2"/>
@@ -3871,8 +4015,9 @@
       <c r="W82" s="2"/>
       <c r="X82" s="2"/>
       <c r="Y82" s="2"/>
-    </row>
-    <row r="83" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z82" s="2"/>
+    </row>
+    <row r="83" spans="1:26" ht="15.75" customHeight="1">
       <c r="A83" s="2"/>
       <c r="B83" s="2"/>
       <c r="C83" s="2"/>
@@ -3898,8 +4043,9 @@
       <c r="W83" s="2"/>
       <c r="X83" s="2"/>
       <c r="Y83" s="2"/>
-    </row>
-    <row r="84" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z83" s="2"/>
+    </row>
+    <row r="84" spans="1:26" ht="15.75" customHeight="1">
       <c r="A84" s="2"/>
       <c r="B84" s="2"/>
       <c r="C84" s="2"/>
@@ -3925,8 +4071,9 @@
       <c r="W84" s="2"/>
       <c r="X84" s="2"/>
       <c r="Y84" s="2"/>
-    </row>
-    <row r="85" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z84" s="2"/>
+    </row>
+    <row r="85" spans="1:26" ht="15.75" customHeight="1">
       <c r="A85" s="2"/>
       <c r="B85" s="2"/>
       <c r="C85" s="2"/>
@@ -3952,8 +4099,9 @@
       <c r="W85" s="2"/>
       <c r="X85" s="2"/>
       <c r="Y85" s="2"/>
-    </row>
-    <row r="86" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z85" s="2"/>
+    </row>
+    <row r="86" spans="1:26" ht="15.75" customHeight="1">
       <c r="A86" s="2"/>
       <c r="B86" s="2"/>
       <c r="C86" s="2"/>
@@ -3979,8 +4127,9 @@
       <c r="W86" s="2"/>
       <c r="X86" s="2"/>
       <c r="Y86" s="2"/>
-    </row>
-    <row r="87" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z86" s="2"/>
+    </row>
+    <row r="87" spans="1:26" ht="15.75" customHeight="1">
       <c r="A87" s="2"/>
       <c r="B87" s="2"/>
       <c r="C87" s="2"/>
@@ -4006,8 +4155,9 @@
       <c r="W87" s="2"/>
       <c r="X87" s="2"/>
       <c r="Y87" s="2"/>
-    </row>
-    <row r="88" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z87" s="2"/>
+    </row>
+    <row r="88" spans="1:26" ht="15.75" customHeight="1">
       <c r="A88" s="2"/>
       <c r="B88" s="2"/>
       <c r="C88" s="2"/>
@@ -4033,8 +4183,9 @@
       <c r="W88" s="2"/>
       <c r="X88" s="2"/>
       <c r="Y88" s="2"/>
-    </row>
-    <row r="89" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z88" s="2"/>
+    </row>
+    <row r="89" spans="1:26" ht="15.75" customHeight="1">
       <c r="A89" s="2"/>
       <c r="B89" s="2"/>
       <c r="C89" s="2"/>
@@ -4060,8 +4211,9 @@
       <c r="W89" s="2"/>
       <c r="X89" s="2"/>
       <c r="Y89" s="2"/>
-    </row>
-    <row r="90" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z89" s="2"/>
+    </row>
+    <row r="90" spans="1:26" ht="15.75" customHeight="1">
       <c r="A90" s="2"/>
       <c r="B90" s="2"/>
       <c r="C90" s="2"/>
@@ -4087,8 +4239,9 @@
       <c r="W90" s="2"/>
       <c r="X90" s="2"/>
       <c r="Y90" s="2"/>
-    </row>
-    <row r="91" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z90" s="2"/>
+    </row>
+    <row r="91" spans="1:26" ht="15.75" customHeight="1">
       <c r="A91" s="2"/>
       <c r="B91" s="2"/>
       <c r="C91" s="2"/>
@@ -4114,8 +4267,9 @@
       <c r="W91" s="2"/>
       <c r="X91" s="2"/>
       <c r="Y91" s="2"/>
-    </row>
-    <row r="92" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z91" s="2"/>
+    </row>
+    <row r="92" spans="1:26" ht="15.75" customHeight="1">
       <c r="A92" s="2"/>
       <c r="B92" s="2"/>
       <c r="C92" s="2"/>
@@ -4141,8 +4295,9 @@
       <c r="W92" s="2"/>
       <c r="X92" s="2"/>
       <c r="Y92" s="2"/>
-    </row>
-    <row r="93" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z92" s="2"/>
+    </row>
+    <row r="93" spans="1:26" ht="15.75" customHeight="1">
       <c r="A93" s="2"/>
       <c r="B93" s="2"/>
       <c r="C93" s="2"/>
@@ -4168,8 +4323,9 @@
       <c r="W93" s="2"/>
       <c r="X93" s="2"/>
       <c r="Y93" s="2"/>
-    </row>
-    <row r="94" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z93" s="2"/>
+    </row>
+    <row r="94" spans="1:26" ht="15.75" customHeight="1">
       <c r="A94" s="2"/>
       <c r="B94" s="2"/>
       <c r="C94" s="2"/>
@@ -4195,8 +4351,9 @@
       <c r="W94" s="2"/>
       <c r="X94" s="2"/>
       <c r="Y94" s="2"/>
-    </row>
-    <row r="95" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z94" s="2"/>
+    </row>
+    <row r="95" spans="1:26" ht="15.75" customHeight="1">
       <c r="A95" s="2"/>
       <c r="B95" s="2"/>
       <c r="C95" s="2"/>
@@ -4222,8 +4379,9 @@
       <c r="W95" s="2"/>
       <c r="X95" s="2"/>
       <c r="Y95" s="2"/>
-    </row>
-    <row r="96" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z95" s="2"/>
+    </row>
+    <row r="96" spans="1:26" ht="15.75" customHeight="1">
       <c r="A96" s="2"/>
       <c r="B96" s="2"/>
       <c r="C96" s="2"/>
@@ -4249,8 +4407,9 @@
       <c r="W96" s="2"/>
       <c r="X96" s="2"/>
       <c r="Y96" s="2"/>
-    </row>
-    <row r="97" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z96" s="2"/>
+    </row>
+    <row r="97" spans="1:26" ht="15.75" customHeight="1">
       <c r="A97" s="2"/>
       <c r="B97" s="2"/>
       <c r="C97" s="2"/>
@@ -4276,8 +4435,9 @@
       <c r="W97" s="2"/>
       <c r="X97" s="2"/>
       <c r="Y97" s="2"/>
-    </row>
-    <row r="98" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z97" s="2"/>
+    </row>
+    <row r="98" spans="1:26" ht="15.75" customHeight="1">
       <c r="A98" s="2"/>
       <c r="B98" s="2"/>
       <c r="C98" s="2"/>
@@ -4303,8 +4463,9 @@
       <c r="W98" s="2"/>
       <c r="X98" s="2"/>
       <c r="Y98" s="2"/>
-    </row>
-    <row r="99" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z98" s="2"/>
+    </row>
+    <row r="99" spans="1:26" ht="15.75" customHeight="1">
       <c r="A99" s="2"/>
       <c r="B99" s="2"/>
       <c r="C99" s="2"/>
@@ -4330,8 +4491,9 @@
       <c r="W99" s="2"/>
       <c r="X99" s="2"/>
       <c r="Y99" s="2"/>
-    </row>
-    <row r="100" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z99" s="2"/>
+    </row>
+    <row r="100" spans="1:26" ht="15.75" customHeight="1">
       <c r="A100" s="2"/>
       <c r="B100" s="2"/>
       <c r="C100" s="2"/>
@@ -4357,8 +4519,9 @@
       <c r="W100" s="2"/>
       <c r="X100" s="2"/>
       <c r="Y100" s="2"/>
-    </row>
-    <row r="101" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z100" s="2"/>
+    </row>
+    <row r="101" spans="1:26" ht="15.75" customHeight="1">
       <c r="A101" s="2"/>
       <c r="B101" s="2"/>
       <c r="C101" s="2"/>
@@ -4384,8 +4547,9 @@
       <c r="W101" s="2"/>
       <c r="X101" s="2"/>
       <c r="Y101" s="2"/>
-    </row>
-    <row r="102" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z101" s="2"/>
+    </row>
+    <row r="102" spans="1:26" ht="15.75" customHeight="1">
       <c r="A102" s="2"/>
       <c r="B102" s="2"/>
       <c r="C102" s="2"/>
@@ -4411,8 +4575,9 @@
       <c r="W102" s="2"/>
       <c r="X102" s="2"/>
       <c r="Y102" s="2"/>
-    </row>
-    <row r="103" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z102" s="2"/>
+    </row>
+    <row r="103" spans="1:26" ht="15.75" customHeight="1">
       <c r="A103" s="2"/>
       <c r="B103" s="2"/>
       <c r="C103" s="2"/>
@@ -4438,8 +4603,9 @@
       <c r="W103" s="2"/>
       <c r="X103" s="2"/>
       <c r="Y103" s="2"/>
-    </row>
-    <row r="104" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z103" s="2"/>
+    </row>
+    <row r="104" spans="1:26" ht="15.75" customHeight="1">
       <c r="A104" s="2"/>
       <c r="B104" s="2"/>
       <c r="C104" s="2"/>
@@ -4465,8 +4631,9 @@
       <c r="W104" s="2"/>
       <c r="X104" s="2"/>
       <c r="Y104" s="2"/>
-    </row>
-    <row r="105" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z104" s="2"/>
+    </row>
+    <row r="105" spans="1:26" ht="15.75" customHeight="1">
       <c r="A105" s="2"/>
       <c r="B105" s="2"/>
       <c r="C105" s="2"/>
@@ -4492,8 +4659,9 @@
       <c r="W105" s="2"/>
       <c r="X105" s="2"/>
       <c r="Y105" s="2"/>
-    </row>
-    <row r="106" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z105" s="2"/>
+    </row>
+    <row r="106" spans="1:26" ht="15.75" customHeight="1">
       <c r="A106" s="2"/>
       <c r="B106" s="2"/>
       <c r="C106" s="2"/>
@@ -4519,8 +4687,9 @@
       <c r="W106" s="2"/>
       <c r="X106" s="2"/>
       <c r="Y106" s="2"/>
-    </row>
-    <row r="107" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z106" s="2"/>
+    </row>
+    <row r="107" spans="1:26" ht="15.75" customHeight="1">
       <c r="A107" s="2"/>
       <c r="B107" s="2"/>
       <c r="C107" s="2"/>
@@ -4546,8 +4715,9 @@
       <c r="W107" s="2"/>
       <c r="X107" s="2"/>
       <c r="Y107" s="2"/>
-    </row>
-    <row r="108" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z107" s="2"/>
+    </row>
+    <row r="108" spans="1:26" ht="15.75" customHeight="1">
       <c r="A108" s="2"/>
       <c r="B108" s="2"/>
       <c r="C108" s="2"/>
@@ -4573,8 +4743,9 @@
       <c r="W108" s="2"/>
       <c r="X108" s="2"/>
       <c r="Y108" s="2"/>
-    </row>
-    <row r="109" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z108" s="2"/>
+    </row>
+    <row r="109" spans="1:26" ht="15.75" customHeight="1">
       <c r="A109" s="2"/>
       <c r="B109" s="2"/>
       <c r="C109" s="2"/>
@@ -4600,8 +4771,9 @@
       <c r="W109" s="2"/>
       <c r="X109" s="2"/>
       <c r="Y109" s="2"/>
-    </row>
-    <row r="110" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z109" s="2"/>
+    </row>
+    <row r="110" spans="1:26" ht="15.75" customHeight="1">
       <c r="A110" s="2"/>
       <c r="B110" s="2"/>
       <c r="C110" s="2"/>
@@ -4627,8 +4799,9 @@
       <c r="W110" s="2"/>
       <c r="X110" s="2"/>
       <c r="Y110" s="2"/>
-    </row>
-    <row r="111" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z110" s="2"/>
+    </row>
+    <row r="111" spans="1:26" ht="15.75" customHeight="1">
       <c r="A111" s="2"/>
       <c r="B111" s="2"/>
       <c r="C111" s="2"/>
@@ -4654,8 +4827,9 @@
       <c r="W111" s="2"/>
       <c r="X111" s="2"/>
       <c r="Y111" s="2"/>
-    </row>
-    <row r="112" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z111" s="2"/>
+    </row>
+    <row r="112" spans="1:26" ht="15.75" customHeight="1">
       <c r="A112" s="2"/>
       <c r="B112" s="2"/>
       <c r="C112" s="2"/>
@@ -4681,8 +4855,9 @@
       <c r="W112" s="2"/>
       <c r="X112" s="2"/>
       <c r="Y112" s="2"/>
-    </row>
-    <row r="113" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z112" s="2"/>
+    </row>
+    <row r="113" spans="1:26" ht="15.75" customHeight="1">
       <c r="A113" s="2"/>
       <c r="B113" s="2"/>
       <c r="C113" s="2"/>
@@ -4708,8 +4883,9 @@
       <c r="W113" s="2"/>
       <c r="X113" s="2"/>
       <c r="Y113" s="2"/>
-    </row>
-    <row r="114" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z113" s="2"/>
+    </row>
+    <row r="114" spans="1:26" ht="15.75" customHeight="1">
       <c r="A114" s="2"/>
       <c r="B114" s="2"/>
       <c r="C114" s="2"/>
@@ -4735,8 +4911,9 @@
       <c r="W114" s="2"/>
       <c r="X114" s="2"/>
       <c r="Y114" s="2"/>
-    </row>
-    <row r="115" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z114" s="2"/>
+    </row>
+    <row r="115" spans="1:26" ht="15.75" customHeight="1">
       <c r="A115" s="2"/>
       <c r="B115" s="2"/>
       <c r="C115" s="2"/>
@@ -4762,8 +4939,9 @@
       <c r="W115" s="2"/>
       <c r="X115" s="2"/>
       <c r="Y115" s="2"/>
-    </row>
-    <row r="116" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z115" s="2"/>
+    </row>
+    <row r="116" spans="1:26" ht="15.75" customHeight="1">
       <c r="A116" s="2"/>
       <c r="B116" s="2"/>
       <c r="C116" s="2"/>
@@ -4789,8 +4967,9 @@
       <c r="W116" s="2"/>
       <c r="X116" s="2"/>
       <c r="Y116" s="2"/>
-    </row>
-    <row r="117" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z116" s="2"/>
+    </row>
+    <row r="117" spans="1:26" ht="15.75" customHeight="1">
       <c r="A117" s="2"/>
       <c r="B117" s="2"/>
       <c r="C117" s="2"/>
@@ -4816,8 +4995,9 @@
       <c r="W117" s="2"/>
       <c r="X117" s="2"/>
       <c r="Y117" s="2"/>
-    </row>
-    <row r="118" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z117" s="2"/>
+    </row>
+    <row r="118" spans="1:26" ht="15.75" customHeight="1">
       <c r="A118" s="2"/>
       <c r="B118" s="2"/>
       <c r="C118" s="2"/>
@@ -4843,8 +5023,9 @@
       <c r="W118" s="2"/>
       <c r="X118" s="2"/>
       <c r="Y118" s="2"/>
-    </row>
-    <row r="119" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z118" s="2"/>
+    </row>
+    <row r="119" spans="1:26" ht="15.75" customHeight="1">
       <c r="A119" s="2"/>
       <c r="B119" s="2"/>
       <c r="C119" s="2"/>
@@ -4870,8 +5051,9 @@
       <c r="W119" s="2"/>
       <c r="X119" s="2"/>
       <c r="Y119" s="2"/>
-    </row>
-    <row r="120" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z119" s="2"/>
+    </row>
+    <row r="120" spans="1:26" ht="15.75" customHeight="1">
       <c r="A120" s="2"/>
       <c r="B120" s="2"/>
       <c r="C120" s="2"/>
@@ -4897,8 +5079,9 @@
       <c r="W120" s="2"/>
       <c r="X120" s="2"/>
       <c r="Y120" s="2"/>
-    </row>
-    <row r="121" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z120" s="2"/>
+    </row>
+    <row r="121" spans="1:26" ht="15.75" customHeight="1">
       <c r="A121" s="2"/>
       <c r="B121" s="2"/>
       <c r="C121" s="2"/>
@@ -4924,8 +5107,9 @@
       <c r="W121" s="2"/>
       <c r="X121" s="2"/>
       <c r="Y121" s="2"/>
-    </row>
-    <row r="122" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z121" s="2"/>
+    </row>
+    <row r="122" spans="1:26" ht="15.75" customHeight="1">
       <c r="A122" s="2"/>
       <c r="B122" s="2"/>
       <c r="C122" s="2"/>
@@ -4951,8 +5135,9 @@
       <c r="W122" s="2"/>
       <c r="X122" s="2"/>
       <c r="Y122" s="2"/>
-    </row>
-    <row r="123" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z122" s="2"/>
+    </row>
+    <row r="123" spans="1:26" ht="15.75" customHeight="1">
       <c r="A123" s="2"/>
       <c r="B123" s="2"/>
       <c r="C123" s="2"/>
@@ -4978,8 +5163,9 @@
       <c r="W123" s="2"/>
       <c r="X123" s="2"/>
       <c r="Y123" s="2"/>
-    </row>
-    <row r="124" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z123" s="2"/>
+    </row>
+    <row r="124" spans="1:26" ht="15.75" customHeight="1">
       <c r="A124" s="2"/>
       <c r="B124" s="2"/>
       <c r="C124" s="2"/>
@@ -5005,8 +5191,9 @@
       <c r="W124" s="2"/>
       <c r="X124" s="2"/>
       <c r="Y124" s="2"/>
-    </row>
-    <row r="125" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z124" s="2"/>
+    </row>
+    <row r="125" spans="1:26" ht="15.75" customHeight="1">
       <c r="A125" s="2"/>
       <c r="B125" s="2"/>
       <c r="C125" s="2"/>
@@ -5032,8 +5219,9 @@
       <c r="W125" s="2"/>
       <c r="X125" s="2"/>
       <c r="Y125" s="2"/>
-    </row>
-    <row r="126" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z125" s="2"/>
+    </row>
+    <row r="126" spans="1:26" ht="15.75" customHeight="1">
       <c r="A126" s="2"/>
       <c r="B126" s="2"/>
       <c r="C126" s="2"/>
@@ -5059,8 +5247,9 @@
       <c r="W126" s="2"/>
       <c r="X126" s="2"/>
       <c r="Y126" s="2"/>
-    </row>
-    <row r="127" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z126" s="2"/>
+    </row>
+    <row r="127" spans="1:26" ht="15.75" customHeight="1">
       <c r="A127" s="2"/>
       <c r="B127" s="2"/>
       <c r="C127" s="2"/>
@@ -5086,8 +5275,9 @@
       <c r="W127" s="2"/>
       <c r="X127" s="2"/>
       <c r="Y127" s="2"/>
-    </row>
-    <row r="128" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z127" s="2"/>
+    </row>
+    <row r="128" spans="1:26" ht="15.75" customHeight="1">
       <c r="A128" s="2"/>
       <c r="B128" s="2"/>
       <c r="C128" s="2"/>
@@ -5113,8 +5303,9 @@
       <c r="W128" s="2"/>
       <c r="X128" s="2"/>
       <c r="Y128" s="2"/>
-    </row>
-    <row r="129" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z128" s="2"/>
+    </row>
+    <row r="129" spans="1:26" ht="15.75" customHeight="1">
       <c r="A129" s="2"/>
       <c r="B129" s="2"/>
       <c r="C129" s="2"/>
@@ -5140,8 +5331,9 @@
       <c r="W129" s="2"/>
       <c r="X129" s="2"/>
       <c r="Y129" s="2"/>
-    </row>
-    <row r="130" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z129" s="2"/>
+    </row>
+    <row r="130" spans="1:26" ht="15.75" customHeight="1">
       <c r="A130" s="2"/>
       <c r="B130" s="2"/>
       <c r="C130" s="2"/>
@@ -5167,8 +5359,9 @@
       <c r="W130" s="2"/>
       <c r="X130" s="2"/>
       <c r="Y130" s="2"/>
-    </row>
-    <row r="131" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z130" s="2"/>
+    </row>
+    <row r="131" spans="1:26" ht="15.75" customHeight="1">
       <c r="A131" s="2"/>
       <c r="B131" s="2"/>
       <c r="C131" s="2"/>
@@ -5194,8 +5387,9 @@
       <c r="W131" s="2"/>
       <c r="X131" s="2"/>
       <c r="Y131" s="2"/>
-    </row>
-    <row r="132" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z131" s="2"/>
+    </row>
+    <row r="132" spans="1:26" ht="15.75" customHeight="1">
       <c r="A132" s="2"/>
       <c r="B132" s="2"/>
       <c r="C132" s="2"/>
@@ -5221,8 +5415,9 @@
       <c r="W132" s="2"/>
       <c r="X132" s="2"/>
       <c r="Y132" s="2"/>
-    </row>
-    <row r="133" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z132" s="2"/>
+    </row>
+    <row r="133" spans="1:26" ht="15.75" customHeight="1">
       <c r="A133" s="2"/>
       <c r="B133" s="2"/>
       <c r="C133" s="2"/>
@@ -5248,8 +5443,9 @@
       <c r="W133" s="2"/>
       <c r="X133" s="2"/>
       <c r="Y133" s="2"/>
-    </row>
-    <row r="134" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z133" s="2"/>
+    </row>
+    <row r="134" spans="1:26" ht="15.75" customHeight="1">
       <c r="A134" s="2"/>
       <c r="B134" s="2"/>
       <c r="C134" s="2"/>
@@ -5275,8 +5471,9 @@
       <c r="W134" s="2"/>
       <c r="X134" s="2"/>
       <c r="Y134" s="2"/>
-    </row>
-    <row r="135" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z134" s="2"/>
+    </row>
+    <row r="135" spans="1:26" ht="15.75" customHeight="1">
       <c r="A135" s="2"/>
       <c r="B135" s="2"/>
       <c r="C135" s="2"/>
@@ -5302,8 +5499,9 @@
       <c r="W135" s="2"/>
       <c r="X135" s="2"/>
       <c r="Y135" s="2"/>
-    </row>
-    <row r="136" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z135" s="2"/>
+    </row>
+    <row r="136" spans="1:26" ht="15.75" customHeight="1">
       <c r="A136" s="2"/>
       <c r="B136" s="2"/>
       <c r="C136" s="2"/>
@@ -5329,8 +5527,9 @@
       <c r="W136" s="2"/>
       <c r="X136" s="2"/>
       <c r="Y136" s="2"/>
-    </row>
-    <row r="137" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z136" s="2"/>
+    </row>
+    <row r="137" spans="1:26" ht="15.75" customHeight="1">
       <c r="A137" s="2"/>
       <c r="B137" s="2"/>
       <c r="C137" s="2"/>
@@ -5356,8 +5555,9 @@
       <c r="W137" s="2"/>
       <c r="X137" s="2"/>
       <c r="Y137" s="2"/>
-    </row>
-    <row r="138" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z137" s="2"/>
+    </row>
+    <row r="138" spans="1:26" ht="15.75" customHeight="1">
       <c r="A138" s="2"/>
       <c r="B138" s="2"/>
       <c r="C138" s="2"/>
@@ -5383,8 +5583,9 @@
       <c r="W138" s="2"/>
       <c r="X138" s="2"/>
       <c r="Y138" s="2"/>
-    </row>
-    <row r="139" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z138" s="2"/>
+    </row>
+    <row r="139" spans="1:26" ht="15.75" customHeight="1">
       <c r="A139" s="2"/>
       <c r="B139" s="2"/>
       <c r="C139" s="2"/>
@@ -5410,8 +5611,9 @@
       <c r="W139" s="2"/>
       <c r="X139" s="2"/>
       <c r="Y139" s="2"/>
-    </row>
-    <row r="140" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z139" s="2"/>
+    </row>
+    <row r="140" spans="1:26" ht="15.75" customHeight="1">
       <c r="A140" s="2"/>
       <c r="B140" s="2"/>
       <c r="C140" s="2"/>
@@ -5437,8 +5639,9 @@
       <c r="W140" s="2"/>
       <c r="X140" s="2"/>
       <c r="Y140" s="2"/>
-    </row>
-    <row r="141" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z140" s="2"/>
+    </row>
+    <row r="141" spans="1:26" ht="15.75" customHeight="1">
       <c r="A141" s="2"/>
       <c r="B141" s="2"/>
       <c r="C141" s="2"/>
@@ -5464,8 +5667,9 @@
       <c r="W141" s="2"/>
       <c r="X141" s="2"/>
       <c r="Y141" s="2"/>
-    </row>
-    <row r="142" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z141" s="2"/>
+    </row>
+    <row r="142" spans="1:26" ht="15.75" customHeight="1">
       <c r="A142" s="2"/>
       <c r="B142" s="2"/>
       <c r="C142" s="2"/>
@@ -5491,8 +5695,9 @@
       <c r="W142" s="2"/>
       <c r="X142" s="2"/>
       <c r="Y142" s="2"/>
-    </row>
-    <row r="143" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z142" s="2"/>
+    </row>
+    <row r="143" spans="1:26" ht="15.75" customHeight="1">
       <c r="A143" s="2"/>
       <c r="B143" s="2"/>
       <c r="C143" s="2"/>
@@ -5518,8 +5723,9 @@
       <c r="W143" s="2"/>
       <c r="X143" s="2"/>
       <c r="Y143" s="2"/>
-    </row>
-    <row r="144" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z143" s="2"/>
+    </row>
+    <row r="144" spans="1:26" ht="15.75" customHeight="1">
       <c r="A144" s="2"/>
       <c r="B144" s="2"/>
       <c r="C144" s="2"/>
@@ -5545,8 +5751,9 @@
       <c r="W144" s="2"/>
       <c r="X144" s="2"/>
       <c r="Y144" s="2"/>
-    </row>
-    <row r="145" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z144" s="2"/>
+    </row>
+    <row r="145" spans="1:26" ht="15.75" customHeight="1">
       <c r="A145" s="2"/>
       <c r="B145" s="2"/>
       <c r="C145" s="2"/>
@@ -5572,8 +5779,9 @@
       <c r="W145" s="2"/>
       <c r="X145" s="2"/>
       <c r="Y145" s="2"/>
-    </row>
-    <row r="146" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z145" s="2"/>
+    </row>
+    <row r="146" spans="1:26" ht="15.75" customHeight="1">
       <c r="A146" s="2"/>
       <c r="B146" s="2"/>
       <c r="C146" s="2"/>
@@ -5599,8 +5807,9 @@
       <c r="W146" s="2"/>
       <c r="X146" s="2"/>
       <c r="Y146" s="2"/>
-    </row>
-    <row r="147" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z146" s="2"/>
+    </row>
+    <row r="147" spans="1:26" ht="15.75" customHeight="1">
       <c r="A147" s="2"/>
       <c r="B147" s="2"/>
       <c r="C147" s="2"/>
@@ -5626,8 +5835,9 @@
       <c r="W147" s="2"/>
       <c r="X147" s="2"/>
       <c r="Y147" s="2"/>
-    </row>
-    <row r="148" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z147" s="2"/>
+    </row>
+    <row r="148" spans="1:26" ht="15.75" customHeight="1">
       <c r="A148" s="2"/>
       <c r="B148" s="2"/>
       <c r="C148" s="2"/>
@@ -5653,8 +5863,9 @@
       <c r="W148" s="2"/>
       <c r="X148" s="2"/>
       <c r="Y148" s="2"/>
-    </row>
-    <row r="149" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z148" s="2"/>
+    </row>
+    <row r="149" spans="1:26" ht="15.75" customHeight="1">
       <c r="A149" s="2"/>
       <c r="B149" s="2"/>
       <c r="C149" s="2"/>
@@ -5680,8 +5891,9 @@
       <c r="W149" s="2"/>
       <c r="X149" s="2"/>
       <c r="Y149" s="2"/>
-    </row>
-    <row r="150" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z149" s="2"/>
+    </row>
+    <row r="150" spans="1:26" ht="15.75" customHeight="1">
       <c r="A150" s="2"/>
       <c r="B150" s="2"/>
       <c r="C150" s="2"/>
@@ -5707,8 +5919,9 @@
       <c r="W150" s="2"/>
       <c r="X150" s="2"/>
       <c r="Y150" s="2"/>
-    </row>
-    <row r="151" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z150" s="2"/>
+    </row>
+    <row r="151" spans="1:26" ht="15.75" customHeight="1">
       <c r="A151" s="2"/>
       <c r="B151" s="2"/>
       <c r="C151" s="2"/>
@@ -5734,8 +5947,9 @@
       <c r="W151" s="2"/>
       <c r="X151" s="2"/>
       <c r="Y151" s="2"/>
-    </row>
-    <row r="152" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z151" s="2"/>
+    </row>
+    <row r="152" spans="1:26" ht="15.75" customHeight="1">
       <c r="A152" s="2"/>
       <c r="B152" s="2"/>
       <c r="C152" s="2"/>
@@ -5761,8 +5975,9 @@
       <c r="W152" s="2"/>
       <c r="X152" s="2"/>
       <c r="Y152" s="2"/>
-    </row>
-    <row r="153" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z152" s="2"/>
+    </row>
+    <row r="153" spans="1:26" ht="15.75" customHeight="1">
       <c r="A153" s="2"/>
       <c r="B153" s="2"/>
       <c r="C153" s="2"/>
@@ -5788,8 +6003,9 @@
       <c r="W153" s="2"/>
       <c r="X153" s="2"/>
       <c r="Y153" s="2"/>
-    </row>
-    <row r="154" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z153" s="2"/>
+    </row>
+    <row r="154" spans="1:26" ht="15.75" customHeight="1">
       <c r="A154" s="2"/>
       <c r="B154" s="2"/>
       <c r="C154" s="2"/>
@@ -5815,8 +6031,9 @@
       <c r="W154" s="2"/>
       <c r="X154" s="2"/>
       <c r="Y154" s="2"/>
-    </row>
-    <row r="155" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z154" s="2"/>
+    </row>
+    <row r="155" spans="1:26" ht="15.75" customHeight="1">
       <c r="A155" s="2"/>
       <c r="B155" s="2"/>
       <c r="C155" s="2"/>
@@ -5842,8 +6059,9 @@
       <c r="W155" s="2"/>
       <c r="X155" s="2"/>
       <c r="Y155" s="2"/>
-    </row>
-    <row r="156" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z155" s="2"/>
+    </row>
+    <row r="156" spans="1:26" ht="15.75" customHeight="1">
       <c r="A156" s="2"/>
       <c r="B156" s="2"/>
       <c r="C156" s="2"/>
@@ -5869,8 +6087,9 @@
       <c r="W156" s="2"/>
       <c r="X156" s="2"/>
       <c r="Y156" s="2"/>
-    </row>
-    <row r="157" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z156" s="2"/>
+    </row>
+    <row r="157" spans="1:26" ht="15.75" customHeight="1">
       <c r="A157" s="2"/>
       <c r="B157" s="2"/>
       <c r="C157" s="2"/>
@@ -5896,8 +6115,9 @@
       <c r="W157" s="2"/>
       <c r="X157" s="2"/>
       <c r="Y157" s="2"/>
-    </row>
-    <row r="158" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z157" s="2"/>
+    </row>
+    <row r="158" spans="1:26" ht="15.75" customHeight="1">
       <c r="A158" s="2"/>
       <c r="B158" s="2"/>
       <c r="C158" s="2"/>
@@ -5923,8 +6143,9 @@
       <c r="W158" s="2"/>
       <c r="X158" s="2"/>
       <c r="Y158" s="2"/>
-    </row>
-    <row r="159" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z158" s="2"/>
+    </row>
+    <row r="159" spans="1:26" ht="15.75" customHeight="1">
       <c r="A159" s="2"/>
       <c r="B159" s="2"/>
       <c r="C159" s="2"/>
@@ -5950,8 +6171,9 @@
       <c r="W159" s="2"/>
       <c r="X159" s="2"/>
       <c r="Y159" s="2"/>
-    </row>
-    <row r="160" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z159" s="2"/>
+    </row>
+    <row r="160" spans="1:26" ht="15.75" customHeight="1">
       <c r="A160" s="2"/>
       <c r="B160" s="2"/>
       <c r="C160" s="2"/>
@@ -5977,8 +6199,9 @@
       <c r="W160" s="2"/>
       <c r="X160" s="2"/>
       <c r="Y160" s="2"/>
-    </row>
-    <row r="161" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z160" s="2"/>
+    </row>
+    <row r="161" spans="1:26" ht="15.75" customHeight="1">
       <c r="A161" s="2"/>
       <c r="B161" s="2"/>
       <c r="C161" s="2"/>
@@ -6004,8 +6227,9 @@
       <c r="W161" s="2"/>
       <c r="X161" s="2"/>
       <c r="Y161" s="2"/>
-    </row>
-    <row r="162" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z161" s="2"/>
+    </row>
+    <row r="162" spans="1:26" ht="15.75" customHeight="1">
       <c r="A162" s="2"/>
       <c r="B162" s="2"/>
       <c r="C162" s="2"/>
@@ -6031,8 +6255,9 @@
       <c r="W162" s="2"/>
       <c r="X162" s="2"/>
       <c r="Y162" s="2"/>
-    </row>
-    <row r="163" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z162" s="2"/>
+    </row>
+    <row r="163" spans="1:26" ht="15.75" customHeight="1">
       <c r="A163" s="2"/>
       <c r="B163" s="2"/>
       <c r="C163" s="2"/>
@@ -6058,8 +6283,9 @@
       <c r="W163" s="2"/>
       <c r="X163" s="2"/>
       <c r="Y163" s="2"/>
-    </row>
-    <row r="164" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z163" s="2"/>
+    </row>
+    <row r="164" spans="1:26" ht="15.75" customHeight="1">
       <c r="A164" s="2"/>
       <c r="B164" s="2"/>
       <c r="C164" s="2"/>
@@ -6085,8 +6311,9 @@
       <c r="W164" s="2"/>
       <c r="X164" s="2"/>
       <c r="Y164" s="2"/>
-    </row>
-    <row r="165" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z164" s="2"/>
+    </row>
+    <row r="165" spans="1:26" ht="15.75" customHeight="1">
       <c r="A165" s="2"/>
       <c r="B165" s="2"/>
       <c r="C165" s="2"/>
@@ -6112,8 +6339,9 @@
       <c r="W165" s="2"/>
       <c r="X165" s="2"/>
       <c r="Y165" s="2"/>
-    </row>
-    <row r="166" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z165" s="2"/>
+    </row>
+    <row r="166" spans="1:26" ht="15.75" customHeight="1">
       <c r="A166" s="2"/>
       <c r="B166" s="2"/>
       <c r="C166" s="2"/>
@@ -6139,8 +6367,9 @@
       <c r="W166" s="2"/>
       <c r="X166" s="2"/>
       <c r="Y166" s="2"/>
-    </row>
-    <row r="167" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z166" s="2"/>
+    </row>
+    <row r="167" spans="1:26" ht="15.75" customHeight="1">
       <c r="A167" s="2"/>
       <c r="B167" s="2"/>
       <c r="C167" s="2"/>
@@ -6166,8 +6395,9 @@
       <c r="W167" s="2"/>
       <c r="X167" s="2"/>
       <c r="Y167" s="2"/>
-    </row>
-    <row r="168" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z167" s="2"/>
+    </row>
+    <row r="168" spans="1:26" ht="15.75" customHeight="1">
       <c r="A168" s="2"/>
       <c r="B168" s="2"/>
       <c r="C168" s="2"/>
@@ -6193,8 +6423,9 @@
       <c r="W168" s="2"/>
       <c r="X168" s="2"/>
       <c r="Y168" s="2"/>
-    </row>
-    <row r="169" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z168" s="2"/>
+    </row>
+    <row r="169" spans="1:26" ht="15.75" customHeight="1">
       <c r="A169" s="2"/>
       <c r="B169" s="2"/>
       <c r="C169" s="2"/>
@@ -6220,8 +6451,9 @@
       <c r="W169" s="2"/>
       <c r="X169" s="2"/>
       <c r="Y169" s="2"/>
-    </row>
-    <row r="170" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z169" s="2"/>
+    </row>
+    <row r="170" spans="1:26" ht="15.75" customHeight="1">
       <c r="A170" s="2"/>
       <c r="B170" s="2"/>
       <c r="C170" s="2"/>
@@ -6247,8 +6479,9 @@
       <c r="W170" s="2"/>
       <c r="X170" s="2"/>
       <c r="Y170" s="2"/>
-    </row>
-    <row r="171" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z170" s="2"/>
+    </row>
+    <row r="171" spans="1:26" ht="15.75" customHeight="1">
       <c r="A171" s="2"/>
       <c r="B171" s="2"/>
       <c r="C171" s="2"/>
@@ -6274,8 +6507,9 @@
       <c r="W171" s="2"/>
       <c r="X171" s="2"/>
       <c r="Y171" s="2"/>
-    </row>
-    <row r="172" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z171" s="2"/>
+    </row>
+    <row r="172" spans="1:26" ht="15.75" customHeight="1">
       <c r="A172" s="2"/>
       <c r="B172" s="2"/>
       <c r="C172" s="2"/>
@@ -6301,8 +6535,9 @@
       <c r="W172" s="2"/>
       <c r="X172" s="2"/>
       <c r="Y172" s="2"/>
-    </row>
-    <row r="173" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z172" s="2"/>
+    </row>
+    <row r="173" spans="1:26" ht="15.75" customHeight="1">
       <c r="A173" s="2"/>
       <c r="B173" s="2"/>
       <c r="C173" s="2"/>
@@ -6328,8 +6563,9 @@
       <c r="W173" s="2"/>
       <c r="X173" s="2"/>
       <c r="Y173" s="2"/>
-    </row>
-    <row r="174" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z173" s="2"/>
+    </row>
+    <row r="174" spans="1:26" ht="15.75" customHeight="1">
       <c r="A174" s="2"/>
       <c r="B174" s="2"/>
       <c r="C174" s="2"/>
@@ -6355,8 +6591,9 @@
       <c r="W174" s="2"/>
       <c r="X174" s="2"/>
       <c r="Y174" s="2"/>
-    </row>
-    <row r="175" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z174" s="2"/>
+    </row>
+    <row r="175" spans="1:26" ht="15.75" customHeight="1">
       <c r="A175" s="2"/>
       <c r="B175" s="2"/>
       <c r="C175" s="2"/>
@@ -6382,8 +6619,9 @@
       <c r="W175" s="2"/>
       <c r="X175" s="2"/>
       <c r="Y175" s="2"/>
-    </row>
-    <row r="176" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z175" s="2"/>
+    </row>
+    <row r="176" spans="1:26" ht="15.75" customHeight="1">
       <c r="A176" s="2"/>
       <c r="B176" s="2"/>
       <c r="C176" s="2"/>
@@ -6409,8 +6647,9 @@
       <c r="W176" s="2"/>
       <c r="X176" s="2"/>
       <c r="Y176" s="2"/>
-    </row>
-    <row r="177" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z176" s="2"/>
+    </row>
+    <row r="177" spans="1:26" ht="15.75" customHeight="1">
       <c r="A177" s="2"/>
       <c r="B177" s="2"/>
       <c r="C177" s="2"/>
@@ -6436,8 +6675,9 @@
       <c r="W177" s="2"/>
       <c r="X177" s="2"/>
       <c r="Y177" s="2"/>
-    </row>
-    <row r="178" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z177" s="2"/>
+    </row>
+    <row r="178" spans="1:26" ht="15.75" customHeight="1">
       <c r="A178" s="2"/>
       <c r="B178" s="2"/>
       <c r="C178" s="2"/>
@@ -6463,8 +6703,9 @@
       <c r="W178" s="2"/>
       <c r="X178" s="2"/>
       <c r="Y178" s="2"/>
-    </row>
-    <row r="179" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z178" s="2"/>
+    </row>
+    <row r="179" spans="1:26" ht="15.75" customHeight="1">
       <c r="A179" s="2"/>
       <c r="B179" s="2"/>
       <c r="C179" s="2"/>
@@ -6490,8 +6731,9 @@
       <c r="W179" s="2"/>
       <c r="X179" s="2"/>
       <c r="Y179" s="2"/>
-    </row>
-    <row r="180" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z179" s="2"/>
+    </row>
+    <row r="180" spans="1:26" ht="15.75" customHeight="1">
       <c r="A180" s="2"/>
       <c r="B180" s="2"/>
       <c r="C180" s="2"/>
@@ -6517,8 +6759,9 @@
       <c r="W180" s="2"/>
       <c r="X180" s="2"/>
       <c r="Y180" s="2"/>
-    </row>
-    <row r="181" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z180" s="2"/>
+    </row>
+    <row r="181" spans="1:26" ht="15.75" customHeight="1">
       <c r="A181" s="2"/>
       <c r="B181" s="2"/>
       <c r="C181" s="2"/>
@@ -6544,8 +6787,9 @@
       <c r="W181" s="2"/>
       <c r="X181" s="2"/>
       <c r="Y181" s="2"/>
-    </row>
-    <row r="182" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z181" s="2"/>
+    </row>
+    <row r="182" spans="1:26" ht="15.75" customHeight="1">
       <c r="A182" s="2"/>
       <c r="B182" s="2"/>
       <c r="C182" s="2"/>
@@ -6571,8 +6815,9 @@
       <c r="W182" s="2"/>
       <c r="X182" s="2"/>
       <c r="Y182" s="2"/>
-    </row>
-    <row r="183" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z182" s="2"/>
+    </row>
+    <row r="183" spans="1:26" ht="15.75" customHeight="1">
       <c r="A183" s="2"/>
       <c r="B183" s="2"/>
       <c r="C183" s="2"/>
@@ -6598,8 +6843,9 @@
       <c r="W183" s="2"/>
       <c r="X183" s="2"/>
       <c r="Y183" s="2"/>
-    </row>
-    <row r="184" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z183" s="2"/>
+    </row>
+    <row r="184" spans="1:26" ht="15.75" customHeight="1">
       <c r="A184" s="2"/>
       <c r="B184" s="2"/>
       <c r="C184" s="2"/>
@@ -6625,8 +6871,9 @@
       <c r="W184" s="2"/>
       <c r="X184" s="2"/>
       <c r="Y184" s="2"/>
-    </row>
-    <row r="185" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z184" s="2"/>
+    </row>
+    <row r="185" spans="1:26" ht="15.75" customHeight="1">
       <c r="A185" s="2"/>
       <c r="B185" s="2"/>
       <c r="C185" s="2"/>
@@ -6652,8 +6899,9 @@
       <c r="W185" s="2"/>
       <c r="X185" s="2"/>
       <c r="Y185" s="2"/>
-    </row>
-    <row r="186" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z185" s="2"/>
+    </row>
+    <row r="186" spans="1:26" ht="15.75" customHeight="1">
       <c r="A186" s="2"/>
       <c r="B186" s="2"/>
       <c r="C186" s="2"/>
@@ -6679,8 +6927,9 @@
       <c r="W186" s="2"/>
       <c r="X186" s="2"/>
       <c r="Y186" s="2"/>
-    </row>
-    <row r="187" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z186" s="2"/>
+    </row>
+    <row r="187" spans="1:26" ht="15.75" customHeight="1">
       <c r="A187" s="2"/>
       <c r="B187" s="2"/>
       <c r="C187" s="2"/>
@@ -6706,8 +6955,9 @@
       <c r="W187" s="2"/>
       <c r="X187" s="2"/>
       <c r="Y187" s="2"/>
-    </row>
-    <row r="188" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z187" s="2"/>
+    </row>
+    <row r="188" spans="1:26" ht="15.75" customHeight="1">
       <c r="A188" s="2"/>
       <c r="B188" s="2"/>
       <c r="C188" s="2"/>
@@ -6733,8 +6983,9 @@
       <c r="W188" s="2"/>
       <c r="X188" s="2"/>
       <c r="Y188" s="2"/>
-    </row>
-    <row r="189" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z188" s="2"/>
+    </row>
+    <row r="189" spans="1:26" ht="15.75" customHeight="1">
       <c r="A189" s="2"/>
       <c r="B189" s="2"/>
       <c r="C189" s="2"/>
@@ -6760,8 +7011,9 @@
       <c r="W189" s="2"/>
       <c r="X189" s="2"/>
       <c r="Y189" s="2"/>
-    </row>
-    <row r="190" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z189" s="2"/>
+    </row>
+    <row r="190" spans="1:26" ht="15.75" customHeight="1">
       <c r="A190" s="2"/>
       <c r="B190" s="2"/>
       <c r="C190" s="2"/>
@@ -6787,8 +7039,9 @@
       <c r="W190" s="2"/>
       <c r="X190" s="2"/>
       <c r="Y190" s="2"/>
-    </row>
-    <row r="191" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z190" s="2"/>
+    </row>
+    <row r="191" spans="1:26" ht="15.75" customHeight="1">
       <c r="A191" s="2"/>
       <c r="B191" s="2"/>
       <c r="C191" s="2"/>
@@ -6814,8 +7067,9 @@
       <c r="W191" s="2"/>
       <c r="X191" s="2"/>
       <c r="Y191" s="2"/>
-    </row>
-    <row r="192" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z191" s="2"/>
+    </row>
+    <row r="192" spans="1:26" ht="15.75" customHeight="1">
       <c r="A192" s="2"/>
       <c r="B192" s="2"/>
       <c r="C192" s="2"/>
@@ -6841,8 +7095,9 @@
       <c r="W192" s="2"/>
       <c r="X192" s="2"/>
       <c r="Y192" s="2"/>
-    </row>
-    <row r="193" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z192" s="2"/>
+    </row>
+    <row r="193" spans="1:26" ht="15.75" customHeight="1">
       <c r="A193" s="2"/>
       <c r="B193" s="2"/>
       <c r="C193" s="2"/>
@@ -6868,8 +7123,9 @@
       <c r="W193" s="2"/>
       <c r="X193" s="2"/>
       <c r="Y193" s="2"/>
-    </row>
-    <row r="194" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z193" s="2"/>
+    </row>
+    <row r="194" spans="1:26" ht="15.75" customHeight="1">
       <c r="A194" s="2"/>
       <c r="B194" s="2"/>
       <c r="C194" s="2"/>
@@ -6895,8 +7151,9 @@
       <c r="W194" s="2"/>
       <c r="X194" s="2"/>
       <c r="Y194" s="2"/>
-    </row>
-    <row r="195" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z194" s="2"/>
+    </row>
+    <row r="195" spans="1:26" ht="15.75" customHeight="1">
       <c r="A195" s="2"/>
       <c r="B195" s="2"/>
       <c r="C195" s="2"/>
@@ -6922,8 +7179,9 @@
       <c r="W195" s="2"/>
       <c r="X195" s="2"/>
       <c r="Y195" s="2"/>
-    </row>
-    <row r="196" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z195" s="2"/>
+    </row>
+    <row r="196" spans="1:26" ht="15.75" customHeight="1">
       <c r="A196" s="2"/>
       <c r="B196" s="2"/>
       <c r="C196" s="2"/>
@@ -6949,8 +7207,9 @@
       <c r="W196" s="2"/>
       <c r="X196" s="2"/>
       <c r="Y196" s="2"/>
-    </row>
-    <row r="197" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z196" s="2"/>
+    </row>
+    <row r="197" spans="1:26" ht="15.75" customHeight="1">
       <c r="A197" s="2"/>
       <c r="B197" s="2"/>
       <c r="C197" s="2"/>
@@ -6976,8 +7235,9 @@
       <c r="W197" s="2"/>
       <c r="X197" s="2"/>
       <c r="Y197" s="2"/>
-    </row>
-    <row r="198" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z197" s="2"/>
+    </row>
+    <row r="198" spans="1:26" ht="15.75" customHeight="1">
       <c r="A198" s="2"/>
       <c r="B198" s="2"/>
       <c r="C198" s="2"/>
@@ -7003,8 +7263,9 @@
       <c r="W198" s="2"/>
       <c r="X198" s="2"/>
       <c r="Y198" s="2"/>
-    </row>
-    <row r="199" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z198" s="2"/>
+    </row>
+    <row r="199" spans="1:26" ht="15.75" customHeight="1">
       <c r="A199" s="2"/>
       <c r="B199" s="2"/>
       <c r="C199" s="2"/>
@@ -7030,8 +7291,9 @@
       <c r="W199" s="2"/>
       <c r="X199" s="2"/>
       <c r="Y199" s="2"/>
-    </row>
-    <row r="200" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z199" s="2"/>
+    </row>
+    <row r="200" spans="1:26" ht="15.75" customHeight="1">
       <c r="A200" s="2"/>
       <c r="B200" s="2"/>
       <c r="C200" s="2"/>
@@ -7057,8 +7319,9 @@
       <c r="W200" s="2"/>
       <c r="X200" s="2"/>
       <c r="Y200" s="2"/>
-    </row>
-    <row r="201" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z200" s="2"/>
+    </row>
+    <row r="201" spans="1:26" ht="15.75" customHeight="1">
       <c r="A201" s="2"/>
       <c r="B201" s="2"/>
       <c r="C201" s="2"/>
@@ -7084,8 +7347,9 @@
       <c r="W201" s="2"/>
       <c r="X201" s="2"/>
       <c r="Y201" s="2"/>
-    </row>
-    <row r="202" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z201" s="2"/>
+    </row>
+    <row r="202" spans="1:26" ht="15.75" customHeight="1">
       <c r="A202" s="2"/>
       <c r="B202" s="2"/>
       <c r="C202" s="2"/>
@@ -7111,8 +7375,9 @@
       <c r="W202" s="2"/>
       <c r="X202" s="2"/>
       <c r="Y202" s="2"/>
-    </row>
-    <row r="203" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z202" s="2"/>
+    </row>
+    <row r="203" spans="1:26" ht="15.75" customHeight="1">
       <c r="A203" s="2"/>
       <c r="B203" s="2"/>
       <c r="C203" s="2"/>
@@ -7138,8 +7403,9 @@
       <c r="W203" s="2"/>
       <c r="X203" s="2"/>
       <c r="Y203" s="2"/>
-    </row>
-    <row r="204" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z203" s="2"/>
+    </row>
+    <row r="204" spans="1:26" ht="15.75" customHeight="1">
       <c r="A204" s="2"/>
       <c r="B204" s="2"/>
       <c r="C204" s="2"/>
@@ -7165,8 +7431,9 @@
       <c r="W204" s="2"/>
       <c r="X204" s="2"/>
       <c r="Y204" s="2"/>
-    </row>
-    <row r="205" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z204" s="2"/>
+    </row>
+    <row r="205" spans="1:26" ht="15.75" customHeight="1">
       <c r="A205" s="2"/>
       <c r="B205" s="2"/>
       <c r="C205" s="2"/>
@@ -7192,8 +7459,9 @@
       <c r="W205" s="2"/>
       <c r="X205" s="2"/>
       <c r="Y205" s="2"/>
-    </row>
-    <row r="206" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z205" s="2"/>
+    </row>
+    <row r="206" spans="1:26" ht="15.75" customHeight="1">
       <c r="A206" s="2"/>
       <c r="B206" s="2"/>
       <c r="C206" s="2"/>
@@ -7219,8 +7487,9 @@
       <c r="W206" s="2"/>
       <c r="X206" s="2"/>
       <c r="Y206" s="2"/>
-    </row>
-    <row r="207" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z206" s="2"/>
+    </row>
+    <row r="207" spans="1:26" ht="15.75" customHeight="1">
       <c r="A207" s="2"/>
       <c r="B207" s="2"/>
       <c r="C207" s="2"/>
@@ -7246,8 +7515,9 @@
       <c r="W207" s="2"/>
       <c r="X207" s="2"/>
       <c r="Y207" s="2"/>
-    </row>
-    <row r="208" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z207" s="2"/>
+    </row>
+    <row r="208" spans="1:26" ht="15.75" customHeight="1">
       <c r="A208" s="2"/>
       <c r="B208" s="2"/>
       <c r="C208" s="2"/>
@@ -7273,8 +7543,9 @@
       <c r="W208" s="2"/>
       <c r="X208" s="2"/>
       <c r="Y208" s="2"/>
-    </row>
-    <row r="209" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z208" s="2"/>
+    </row>
+    <row r="209" spans="1:26" ht="15.75" customHeight="1">
       <c r="A209" s="2"/>
       <c r="B209" s="2"/>
       <c r="C209" s="2"/>
@@ -7300,8 +7571,9 @@
       <c r="W209" s="2"/>
       <c r="X209" s="2"/>
       <c r="Y209" s="2"/>
-    </row>
-    <row r="210" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z209" s="2"/>
+    </row>
+    <row r="210" spans="1:26" ht="15.75" customHeight="1">
       <c r="A210" s="2"/>
       <c r="B210" s="2"/>
       <c r="C210" s="2"/>
@@ -7327,8 +7599,9 @@
       <c r="W210" s="2"/>
       <c r="X210" s="2"/>
       <c r="Y210" s="2"/>
-    </row>
-    <row r="211" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z210" s="2"/>
+    </row>
+    <row r="211" spans="1:26" ht="15.75" customHeight="1">
       <c r="A211" s="2"/>
       <c r="B211" s="2"/>
       <c r="C211" s="2"/>
@@ -7354,8 +7627,9 @@
       <c r="W211" s="2"/>
       <c r="X211" s="2"/>
       <c r="Y211" s="2"/>
-    </row>
-    <row r="212" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z211" s="2"/>
+    </row>
+    <row r="212" spans="1:26" ht="15.75" customHeight="1">
       <c r="A212" s="2"/>
       <c r="B212" s="2"/>
       <c r="C212" s="2"/>
@@ -7381,8 +7655,9 @@
       <c r="W212" s="2"/>
       <c r="X212" s="2"/>
       <c r="Y212" s="2"/>
-    </row>
-    <row r="213" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z212" s="2"/>
+    </row>
+    <row r="213" spans="1:26" ht="15.75" customHeight="1">
       <c r="A213" s="2"/>
       <c r="B213" s="2"/>
       <c r="C213" s="2"/>
@@ -7408,8 +7683,9 @@
       <c r="W213" s="2"/>
       <c r="X213" s="2"/>
       <c r="Y213" s="2"/>
-    </row>
-    <row r="214" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z213" s="2"/>
+    </row>
+    <row r="214" spans="1:26" ht="15.75" customHeight="1">
       <c r="A214" s="2"/>
       <c r="B214" s="2"/>
       <c r="C214" s="2"/>
@@ -7435,8 +7711,9 @@
       <c r="W214" s="2"/>
       <c r="X214" s="2"/>
       <c r="Y214" s="2"/>
-    </row>
-    <row r="215" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z214" s="2"/>
+    </row>
+    <row r="215" spans="1:26" ht="15.75" customHeight="1">
       <c r="A215" s="2"/>
       <c r="B215" s="2"/>
       <c r="C215" s="2"/>
@@ -7462,8 +7739,9 @@
       <c r="W215" s="2"/>
       <c r="X215" s="2"/>
       <c r="Y215" s="2"/>
-    </row>
-    <row r="216" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z215" s="2"/>
+    </row>
+    <row r="216" spans="1:26" ht="15.75" customHeight="1">
       <c r="A216" s="2"/>
       <c r="B216" s="2"/>
       <c r="C216" s="2"/>
@@ -7489,8 +7767,9 @@
       <c r="W216" s="2"/>
       <c r="X216" s="2"/>
       <c r="Y216" s="2"/>
-    </row>
-    <row r="217" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z216" s="2"/>
+    </row>
+    <row r="217" spans="1:26" ht="15.75" customHeight="1">
       <c r="A217" s="2"/>
       <c r="B217" s="2"/>
       <c r="C217" s="2"/>
@@ -7516,8 +7795,9 @@
       <c r="W217" s="2"/>
       <c r="X217" s="2"/>
       <c r="Y217" s="2"/>
-    </row>
-    <row r="218" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z217" s="2"/>
+    </row>
+    <row r="218" spans="1:26" ht="15.75" customHeight="1">
       <c r="A218" s="2"/>
       <c r="B218" s="2"/>
       <c r="C218" s="2"/>
@@ -7543,8 +7823,9 @@
       <c r="W218" s="2"/>
       <c r="X218" s="2"/>
       <c r="Y218" s="2"/>
-    </row>
-    <row r="219" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z218" s="2"/>
+    </row>
+    <row r="219" spans="1:26" ht="15.75" customHeight="1">
       <c r="A219" s="2"/>
       <c r="B219" s="2"/>
       <c r="C219" s="2"/>
@@ -7570,8 +7851,9 @@
       <c r="W219" s="2"/>
       <c r="X219" s="2"/>
       <c r="Y219" s="2"/>
-    </row>
-    <row r="220" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z219" s="2"/>
+    </row>
+    <row r="220" spans="1:26" ht="15.75" customHeight="1">
       <c r="A220" s="2"/>
       <c r="B220" s="2"/>
       <c r="C220" s="2"/>
@@ -7597,8 +7879,9 @@
       <c r="W220" s="2"/>
       <c r="X220" s="2"/>
       <c r="Y220" s="2"/>
-    </row>
-    <row r="221" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z220" s="2"/>
+    </row>
+    <row r="221" spans="1:26" ht="15.75" customHeight="1">
       <c r="A221" s="2"/>
       <c r="B221" s="2"/>
       <c r="C221" s="2"/>
@@ -7624,10 +7907,11 @@
       <c r="W221" s="2"/>
       <c r="X221" s="2"/>
       <c r="Y221" s="2"/>
-    </row>
-    <row r="222" spans="1:25" ht="15.75" customHeight="1"/>
-    <row r="223" spans="1:25" ht="15.75" customHeight="1"/>
-    <row r="224" spans="1:25" ht="15.75" customHeight="1"/>
+      <c r="Z221" s="2"/>
+    </row>
+    <row r="222" spans="1:26" ht="15.75" customHeight="1"/>
+    <row r="223" spans="1:26" ht="15.75" customHeight="1"/>
+    <row r="224" spans="1:26" ht="15.75" customHeight="1"/>
     <row r="225" ht="15.75" customHeight="1"/>
     <row r="226" ht="15.75" customHeight="1"/>
     <row r="227" ht="15.75" customHeight="1"/>
@@ -8421,17 +8705,17 @@
       <formula>"Magas"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K2:K8 K10:K23">
+  <conditionalFormatting sqref="K2:L4 K18:L23 K10:K17 K5:K8 L5:L17">
     <cfRule type="cellIs" dxfId="20" priority="10" operator="equal">
       <formula>"Siker"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K2:K8 K10:K23">
+  <conditionalFormatting sqref="K2:L4 K18:L23 K10:K17 K5:K8 L5:L17">
     <cfRule type="cellIs" dxfId="19" priority="11" operator="equal">
       <formula>"Nem futtatható"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K2:K8 K10:K23">
+  <conditionalFormatting sqref="K2:L4 K18:L23 K10:K17 K5:K8 L5:L17">
     <cfRule type="cellIs" dxfId="18" priority="12" operator="equal">
       <formula>"Hiba"</formula>
     </cfRule>
@@ -8467,7 +8751,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" sqref="K2:K23">
+    <dataValidation type="list" allowBlank="1" sqref="K2:L23">
       <formula1>"Siker,Nem futtatható,Hiba"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" sqref="E2:E23">

</xml_diff>